<commit_message>
Update leave application Excel template and add support for additional leave types
Updated salary field to include 'PHP' prefix and corrected position field to use 'title' instead of 'position_name'. Adjusted date filing cell reference from G14 to F14. Added support for six additional leave types: adoption leave, rehabilitation leave, vacation leave, special leave benefits for women, calamity leave, and VAWC leave. Changed download button from non-functional button element to working anchor link
</commit_message>
<xml_diff>
--- a/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
+++ b/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Marvin File 2024\FORMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source Codes\personal-info-management-system\resources\views\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D8E6B28-8FFC-40CE-88D8-910429789D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96994F0-B4CA-4F76-BAF5-9BA6C9F384E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Civil Service Form No. 6</t>
   </si>
@@ -928,27 +928,12 @@
     <t xml:space="preserve">* For leave of absence for thirty (30) calendar days or more   and terminal leave, application shall be accompanied by a clearance from money, property and   work-related accountabilities (pursuant to CSC Memorandum Circular No. 2, s. 1985). </t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>DEPED/Plaridel CS/Baybay 6</t>
   </si>
   <si>
-    <t>ADMINISTRATIVE AIDE VI</t>
-  </si>
-  <si>
     <t>Feverish and Headache</t>
   </si>
   <si>
-    <t>1 day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MARVIN </t>
-  </si>
-  <si>
-    <t>L.  AREVALO</t>
-  </si>
-  <si>
     <t>JULIUS CESAR L. DE LA CERNA</t>
   </si>
   <si>
@@ -971,15 +956,6 @@
   </si>
   <si>
     <t>SCHOOL HEAD/CLUSTER IN-CHARGE</t>
-  </si>
-  <si>
-    <t>ROBIN</t>
-  </si>
-  <si>
-    <t>PADILLA</t>
-  </si>
-  <si>
-    <t>TAMBIS</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1423,8 +1399,68 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1468,67 +1504,13 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1901,8 +1883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27B6FB-8E85-4B80-9281-508316E41DF7}">
   <dimension ref="A1:WVX123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2950,121 +2932,121 @@
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
-      <c r="N6" s="70"/>
-      <c r="O6" s="70"/>
+      <c r="A6" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="72"/>
-      <c r="O7" s="72"/>
+      <c r="A7" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="70"/>
-      <c r="N8" s="70"/>
-      <c r="O8" s="70"/>
+      <c r="A8" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
     </row>
     <row r="9" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="73"/>
-      <c r="J10" s="73"/>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -3076,44 +3058,38 @@
       <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="74" t="s">
+      <c r="G11" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74" t="s">
+      <c r="H11" s="52"/>
+      <c r="I11" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74" t="s">
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="75"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="G12" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="77"/>
-      <c r="I12" s="77" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="77"/>
-      <c r="K12" s="77"/>
-      <c r="L12" s="77"/>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="O12" s="78"/>
+      <c r="C12" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="56"/>
     </row>
     <row r="13" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
@@ -3138,26 +3114,20 @@
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="12">
-        <v>45506</v>
-      </c>
+      <c r="F14" s="12"/>
       <c r="G14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
       <c r="M14" s="14"/>
       <c r="N14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="15">
-        <v>17553</v>
-      </c>
+      <c r="O14" s="15"/>
     </row>
     <row r="15" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9"/>
@@ -3177,22 +3147,22 @@
     </row>
     <row r="16" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
-      <c r="K17" s="65"/>
-      <c r="L17" s="65"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="66"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="48"/>
     </row>
     <row r="18" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
@@ -3250,9 +3220,7 @@
     </row>
     <row r="22" spans="2:15" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8"/>
-      <c r="C22" s="42" t="s">
-        <v>71</v>
-      </c>
+      <c r="C22" s="42"/>
       <c r="E22" s="21" t="s">
         <v>21</v>
       </c>
@@ -3303,17 +3271,15 @@
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="42" t="s">
-        <v>71</v>
-      </c>
+      <c r="J25" s="42"/>
       <c r="L25" s="21" t="s">
         <v>28</v>
       </c>
       <c r="M25" s="21"/>
-      <c r="N25" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="O25" s="69"/>
+      <c r="N25" s="43" t="s">
+        <v>72</v>
+      </c>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
@@ -3422,8 +3388,8 @@
       <c r="E33" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
       <c r="H33" s="22"/>
       <c r="I33" s="8"/>
       <c r="J33" s="20"/>
@@ -3471,11 +3437,9 @@
     </row>
     <row r="36" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="E36" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="22"/>
       <c r="I36" s="8"/>
       <c r="J36" s="20"/>
@@ -3501,36 +3465,32 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
-      <c r="E38" s="59">
+      <c r="E38" s="58">
         <v>45330</v>
       </c>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="10"/>
-      <c r="K38" s="10"/>
-      <c r="L38" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="M38" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="N38" s="10"/>
-      <c r="O38" s="11"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="80"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="61" t="s">
+      <c r="I39" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="J39" s="62"/>
-      <c r="K39" s="62"/>
-      <c r="L39" s="62"/>
-      <c r="M39" s="62"/>
-      <c r="N39" s="62"/>
-      <c r="O39" s="63"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="62"/>
     </row>
     <row r="40" spans="2:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
@@ -3550,22 +3510,22 @@
     </row>
     <row r="41" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="64" t="s">
+      <c r="B42" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="65"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="65"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="66"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="48"/>
     </row>
     <row r="43" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -3593,8 +3553,8 @@
       <c r="E45" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
       <c r="H45" s="21"/>
       <c r="I45" s="8"/>
       <c r="O45" s="22"/>
@@ -3683,33 +3643,33 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="E53" s="56" t="s">
-        <v>78</v>
-      </c>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
+      <c r="E53" s="76" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
       <c r="I53" s="8"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="56"/>
-      <c r="O53" s="57"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="77"/>
     </row>
     <row r="54" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
-      <c r="E54" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
+      <c r="E54" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
       <c r="I54" s="38"/>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
-      <c r="L54" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="M54" s="48"/>
-      <c r="N54" s="48"/>
-      <c r="O54" s="49"/>
+      <c r="L54" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="69"/>
     </row>
     <row r="55" spans="2:15" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
@@ -3748,9 +3708,9 @@
       <c r="O56" s="27"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="50"/>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="71"/>
       <c r="E57" s="21" t="s">
         <v>64</v>
       </c>
@@ -3789,26 +3749,26 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
-      <c r="G61" s="51" t="s">
-        <v>79</v>
-      </c>
-      <c r="H61" s="51"/>
-      <c r="I61" s="51"/>
-      <c r="J61" s="51"/>
-      <c r="K61" s="51"/>
-      <c r="L61" s="51"/>
+      <c r="G61" s="71" t="s">
+        <v>74</v>
+      </c>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="71"/>
+      <c r="L61" s="71"/>
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
-      <c r="G62" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="H62" s="52"/>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
-      <c r="K62" s="52"/>
-      <c r="L62" s="52"/>
+      <c r="G62" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="H62" s="72"/>
+      <c r="I62" s="72"/>
+      <c r="J62" s="72"/>
+      <c r="K62" s="72"/>
+      <c r="L62" s="72"/>
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3834,731 +3794,731 @@
     <row r="68" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="53" t="s">
+      <c r="B70" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
-      <c r="J70" s="54"/>
-      <c r="K70" s="54"/>
-      <c r="L70" s="54"/>
-      <c r="M70" s="54"/>
-      <c r="N70" s="54"/>
-      <c r="O70" s="55"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="74"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
+      <c r="K70" s="74"/>
+      <c r="L70" s="74"/>
+      <c r="M70" s="74"/>
+      <c r="N70" s="74"/>
+      <c r="O70" s="75"/>
     </row>
     <row r="71" spans="2:15" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="44" t="s">
+      <c r="B72" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
-      <c r="E72" s="45"/>
-      <c r="F72" s="45"/>
-      <c r="G72" s="45"/>
-      <c r="H72" s="45"/>
-      <c r="I72" s="44" t="s">
+      <c r="C72" s="65"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="65"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="J72" s="45"/>
-      <c r="K72" s="45"/>
-      <c r="L72" s="45"/>
-      <c r="M72" s="45"/>
-      <c r="N72" s="45"/>
-      <c r="O72" s="45"/>
+      <c r="J72" s="65"/>
+      <c r="K72" s="65"/>
+      <c r="L72" s="65"/>
+      <c r="M72" s="65"/>
+      <c r="N72" s="65"/>
+      <c r="O72" s="65"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="45"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="45"/>
-      <c r="E73" s="45"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="45"/>
-      <c r="H73" s="45"/>
-      <c r="I73" s="45"/>
-      <c r="J73" s="45"/>
-      <c r="K73" s="45"/>
-      <c r="L73" s="45"/>
-      <c r="M73" s="45"/>
-      <c r="N73" s="45"/>
-      <c r="O73" s="45"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="65"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="65"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="65"/>
+      <c r="L73" s="65"/>
+      <c r="M73" s="65"/>
+      <c r="N73" s="65"/>
+      <c r="O73" s="65"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="45"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45"/>
-      <c r="E74" s="45"/>
-      <c r="F74" s="45"/>
-      <c r="G74" s="45"/>
-      <c r="H74" s="45"/>
-      <c r="I74" s="45"/>
-      <c r="J74" s="45"/>
-      <c r="K74" s="45"/>
-      <c r="L74" s="45"/>
-      <c r="M74" s="45"/>
-      <c r="N74" s="45"/>
-      <c r="O74" s="45"/>
+      <c r="B74" s="65"/>
+      <c r="C74" s="65"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="65"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="65"/>
+      <c r="J74" s="65"/>
+      <c r="K74" s="65"/>
+      <c r="L74" s="65"/>
+      <c r="M74" s="65"/>
+      <c r="N74" s="65"/>
+      <c r="O74" s="65"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="45"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="45"/>
-      <c r="H75" s="45"/>
-      <c r="I75" s="45"/>
-      <c r="J75" s="45"/>
-      <c r="K75" s="45"/>
-      <c r="L75" s="45"/>
-      <c r="M75" s="45"/>
-      <c r="N75" s="45"/>
-      <c r="O75" s="45"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="65"/>
+      <c r="D75" s="65"/>
+      <c r="E75" s="65"/>
+      <c r="F75" s="65"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="65"/>
+      <c r="J75" s="65"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="65"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="65"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="45"/>
-      <c r="C76" s="45"/>
-      <c r="D76" s="45"/>
-      <c r="E76" s="45"/>
-      <c r="F76" s="45"/>
-      <c r="G76" s="45"/>
-      <c r="H76" s="45"/>
-      <c r="I76" s="45"/>
-      <c r="J76" s="45"/>
-      <c r="K76" s="45"/>
-      <c r="L76" s="45"/>
-      <c r="M76" s="45"/>
-      <c r="N76" s="45"/>
-      <c r="O76" s="45"/>
+      <c r="B76" s="65"/>
+      <c r="C76" s="65"/>
+      <c r="D76" s="65"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="65"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="65"/>
+      <c r="O76" s="65"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="45"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="45"/>
-      <c r="J77" s="45"/>
-      <c r="K77" s="45"/>
-      <c r="L77" s="45"/>
-      <c r="M77" s="45"/>
-      <c r="N77" s="45"/>
-      <c r="O77" s="45"/>
+      <c r="B77" s="65"/>
+      <c r="C77" s="65"/>
+      <c r="D77" s="65"/>
+      <c r="E77" s="65"/>
+      <c r="F77" s="65"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="65"/>
+      <c r="J77" s="65"/>
+      <c r="K77" s="65"/>
+      <c r="L77" s="65"/>
+      <c r="M77" s="65"/>
+      <c r="N77" s="65"/>
+      <c r="O77" s="65"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="45"/>
-      <c r="H78" s="45"/>
-      <c r="I78" s="45"/>
-      <c r="J78" s="45"/>
-      <c r="K78" s="45"/>
-      <c r="L78" s="45"/>
-      <c r="M78" s="45"/>
-      <c r="N78" s="45"/>
-      <c r="O78" s="45"/>
+      <c r="B78" s="65"/>
+      <c r="C78" s="65"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="65"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
+      <c r="J78" s="65"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="65"/>
+      <c r="N78" s="65"/>
+      <c r="O78" s="65"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="45"/>
-      <c r="C79" s="45"/>
-      <c r="D79" s="45"/>
-      <c r="E79" s="45"/>
-      <c r="F79" s="45"/>
-      <c r="G79" s="45"/>
-      <c r="H79" s="45"/>
-      <c r="I79" s="45"/>
-      <c r="J79" s="45"/>
-      <c r="K79" s="45"/>
-      <c r="L79" s="45"/>
-      <c r="M79" s="45"/>
-      <c r="N79" s="45"/>
-      <c r="O79" s="45"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="65"/>
+      <c r="D79" s="65"/>
+      <c r="E79" s="65"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="65"/>
+      <c r="J79" s="65"/>
+      <c r="K79" s="65"/>
+      <c r="L79" s="65"/>
+      <c r="M79" s="65"/>
+      <c r="N79" s="65"/>
+      <c r="O79" s="65"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="45"/>
-      <c r="C80" s="45"/>
-      <c r="D80" s="45"/>
-      <c r="E80" s="45"/>
-      <c r="F80" s="45"/>
-      <c r="G80" s="45"/>
-      <c r="H80" s="45"/>
-      <c r="I80" s="45"/>
-      <c r="J80" s="45"/>
-      <c r="K80" s="45"/>
-      <c r="L80" s="45"/>
-      <c r="M80" s="45"/>
-      <c r="N80" s="45"/>
-      <c r="O80" s="45"/>
+      <c r="B80" s="65"/>
+      <c r="C80" s="65"/>
+      <c r="D80" s="65"/>
+      <c r="E80" s="65"/>
+      <c r="F80" s="65"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
+      <c r="J80" s="65"/>
+      <c r="K80" s="65"/>
+      <c r="L80" s="65"/>
+      <c r="M80" s="65"/>
+      <c r="N80" s="65"/>
+      <c r="O80" s="65"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="45"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="45"/>
-      <c r="E81" s="45"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="45"/>
-      <c r="H81" s="45"/>
-      <c r="I81" s="45"/>
-      <c r="J81" s="45"/>
-      <c r="K81" s="45"/>
-      <c r="L81" s="45"/>
-      <c r="M81" s="45"/>
-      <c r="N81" s="45"/>
-      <c r="O81" s="45"/>
+      <c r="B81" s="65"/>
+      <c r="C81" s="65"/>
+      <c r="D81" s="65"/>
+      <c r="E81" s="65"/>
+      <c r="F81" s="65"/>
+      <c r="G81" s="65"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="65"/>
+      <c r="J81" s="65"/>
+      <c r="K81" s="65"/>
+      <c r="L81" s="65"/>
+      <c r="M81" s="65"/>
+      <c r="N81" s="65"/>
+      <c r="O81" s="65"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="45"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="45"/>
-      <c r="E82" s="45"/>
-      <c r="F82" s="45"/>
-      <c r="G82" s="45"/>
-      <c r="H82" s="45"/>
-      <c r="I82" s="45"/>
-      <c r="J82" s="45"/>
-      <c r="K82" s="45"/>
-      <c r="L82" s="45"/>
-      <c r="M82" s="45"/>
-      <c r="N82" s="45"/>
-      <c r="O82" s="45"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
+      <c r="D82" s="65"/>
+      <c r="E82" s="65"/>
+      <c r="F82" s="65"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="65"/>
+      <c r="J82" s="65"/>
+      <c r="K82" s="65"/>
+      <c r="L82" s="65"/>
+      <c r="M82" s="65"/>
+      <c r="N82" s="65"/>
+      <c r="O82" s="65"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="45"/>
-      <c r="C83" s="45"/>
-      <c r="D83" s="45"/>
-      <c r="E83" s="45"/>
-      <c r="F83" s="45"/>
-      <c r="G83" s="45"/>
-      <c r="H83" s="45"/>
-      <c r="I83" s="45"/>
-      <c r="J83" s="45"/>
-      <c r="K83" s="45"/>
-      <c r="L83" s="45"/>
-      <c r="M83" s="45"/>
-      <c r="N83" s="45"/>
-      <c r="O83" s="45"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="65"/>
+      <c r="D83" s="65"/>
+      <c r="E83" s="65"/>
+      <c r="F83" s="65"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
+      <c r="L83" s="65"/>
+      <c r="M83" s="65"/>
+      <c r="N83" s="65"/>
+      <c r="O83" s="65"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="45"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="45"/>
-      <c r="E84" s="45"/>
-      <c r="F84" s="45"/>
-      <c r="G84" s="45"/>
-      <c r="H84" s="45"/>
-      <c r="I84" s="45"/>
-      <c r="J84" s="45"/>
-      <c r="K84" s="45"/>
-      <c r="L84" s="45"/>
-      <c r="M84" s="45"/>
-      <c r="N84" s="45"/>
-      <c r="O84" s="45"/>
+      <c r="B84" s="65"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="65"/>
+      <c r="E84" s="65"/>
+      <c r="F84" s="65"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="65"/>
+      <c r="J84" s="65"/>
+      <c r="K84" s="65"/>
+      <c r="L84" s="65"/>
+      <c r="M84" s="65"/>
+      <c r="N84" s="65"/>
+      <c r="O84" s="65"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="45"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="45"/>
-      <c r="E85" s="45"/>
-      <c r="F85" s="45"/>
-      <c r="G85" s="45"/>
-      <c r="H85" s="45"/>
-      <c r="I85" s="45"/>
-      <c r="J85" s="45"/>
-      <c r="K85" s="45"/>
-      <c r="L85" s="45"/>
-      <c r="M85" s="45"/>
-      <c r="N85" s="45"/>
-      <c r="O85" s="45"/>
+      <c r="B85" s="65"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="65"/>
+      <c r="E85" s="65"/>
+      <c r="F85" s="65"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="65"/>
+      <c r="M85" s="65"/>
+      <c r="N85" s="65"/>
+      <c r="O85" s="65"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="45"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="45"/>
-      <c r="E86" s="45"/>
-      <c r="F86" s="45"/>
-      <c r="G86" s="45"/>
-      <c r="H86" s="45"/>
-      <c r="I86" s="45"/>
-      <c r="J86" s="45"/>
-      <c r="K86" s="45"/>
-      <c r="L86" s="45"/>
-      <c r="M86" s="45"/>
-      <c r="N86" s="45"/>
-      <c r="O86" s="45"/>
+      <c r="B86" s="65"/>
+      <c r="C86" s="65"/>
+      <c r="D86" s="65"/>
+      <c r="E86" s="65"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="65"/>
+      <c r="M86" s="65"/>
+      <c r="N86" s="65"/>
+      <c r="O86" s="65"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="45"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="45"/>
-      <c r="E87" s="45"/>
-      <c r="F87" s="45"/>
-      <c r="G87" s="45"/>
-      <c r="H87" s="45"/>
-      <c r="I87" s="45"/>
-      <c r="J87" s="45"/>
-      <c r="K87" s="45"/>
-      <c r="L87" s="45"/>
-      <c r="M87" s="45"/>
-      <c r="N87" s="45"/>
-      <c r="O87" s="45"/>
+      <c r="B87" s="65"/>
+      <c r="C87" s="65"/>
+      <c r="D87" s="65"/>
+      <c r="E87" s="65"/>
+      <c r="F87" s="65"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="65"/>
+      <c r="L87" s="65"/>
+      <c r="M87" s="65"/>
+      <c r="N87" s="65"/>
+      <c r="O87" s="65"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="45"/>
-      <c r="C88" s="45"/>
-      <c r="D88" s="45"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="45"/>
-      <c r="G88" s="45"/>
-      <c r="H88" s="45"/>
-      <c r="I88" s="45"/>
-      <c r="J88" s="45"/>
-      <c r="K88" s="45"/>
-      <c r="L88" s="45"/>
-      <c r="M88" s="45"/>
-      <c r="N88" s="45"/>
-      <c r="O88" s="45"/>
+      <c r="B88" s="65"/>
+      <c r="C88" s="65"/>
+      <c r="D88" s="65"/>
+      <c r="E88" s="65"/>
+      <c r="F88" s="65"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="65"/>
+      <c r="J88" s="65"/>
+      <c r="K88" s="65"/>
+      <c r="L88" s="65"/>
+      <c r="M88" s="65"/>
+      <c r="N88" s="65"/>
+      <c r="O88" s="65"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="45"/>
-      <c r="C89" s="45"/>
-      <c r="D89" s="45"/>
-      <c r="E89" s="45"/>
-      <c r="F89" s="45"/>
-      <c r="G89" s="45"/>
-      <c r="H89" s="45"/>
-      <c r="I89" s="45"/>
-      <c r="J89" s="45"/>
-      <c r="K89" s="45"/>
-      <c r="L89" s="45"/>
-      <c r="M89" s="45"/>
-      <c r="N89" s="45"/>
-      <c r="O89" s="45"/>
+      <c r="B89" s="65"/>
+      <c r="C89" s="65"/>
+      <c r="D89" s="65"/>
+      <c r="E89" s="65"/>
+      <c r="F89" s="65"/>
+      <c r="G89" s="65"/>
+      <c r="H89" s="65"/>
+      <c r="I89" s="65"/>
+      <c r="J89" s="65"/>
+      <c r="K89" s="65"/>
+      <c r="L89" s="65"/>
+      <c r="M89" s="65"/>
+      <c r="N89" s="65"/>
+      <c r="O89" s="65"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="45"/>
-      <c r="C90" s="45"/>
-      <c r="D90" s="45"/>
-      <c r="E90" s="45"/>
-      <c r="F90" s="45"/>
-      <c r="G90" s="45"/>
-      <c r="H90" s="45"/>
-      <c r="I90" s="45"/>
-      <c r="J90" s="45"/>
-      <c r="K90" s="45"/>
-      <c r="L90" s="45"/>
-      <c r="M90" s="45"/>
-      <c r="N90" s="45"/>
-      <c r="O90" s="45"/>
+      <c r="B90" s="65"/>
+      <c r="C90" s="65"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="65"/>
+      <c r="F90" s="65"/>
+      <c r="G90" s="65"/>
+      <c r="H90" s="65"/>
+      <c r="I90" s="65"/>
+      <c r="J90" s="65"/>
+      <c r="K90" s="65"/>
+      <c r="L90" s="65"/>
+      <c r="M90" s="65"/>
+      <c r="N90" s="65"/>
+      <c r="O90" s="65"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="45"/>
-      <c r="C91" s="45"/>
-      <c r="D91" s="45"/>
-      <c r="E91" s="45"/>
-      <c r="F91" s="45"/>
-      <c r="G91" s="45"/>
-      <c r="H91" s="45"/>
-      <c r="I91" s="45"/>
-      <c r="J91" s="45"/>
-      <c r="K91" s="45"/>
-      <c r="L91" s="45"/>
-      <c r="M91" s="45"/>
-      <c r="N91" s="45"/>
-      <c r="O91" s="45"/>
+      <c r="B91" s="65"/>
+      <c r="C91" s="65"/>
+      <c r="D91" s="65"/>
+      <c r="E91" s="65"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="65"/>
+      <c r="H91" s="65"/>
+      <c r="I91" s="65"/>
+      <c r="J91" s="65"/>
+      <c r="K91" s="65"/>
+      <c r="L91" s="65"/>
+      <c r="M91" s="65"/>
+      <c r="N91" s="65"/>
+      <c r="O91" s="65"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="45"/>
-      <c r="C92" s="45"/>
-      <c r="D92" s="45"/>
-      <c r="E92" s="45"/>
-      <c r="F92" s="45"/>
-      <c r="G92" s="45"/>
-      <c r="H92" s="45"/>
-      <c r="I92" s="45"/>
-      <c r="J92" s="45"/>
-      <c r="K92" s="45"/>
-      <c r="L92" s="45"/>
-      <c r="M92" s="45"/>
-      <c r="N92" s="45"/>
-      <c r="O92" s="45"/>
+      <c r="B92" s="65"/>
+      <c r="C92" s="65"/>
+      <c r="D92" s="65"/>
+      <c r="E92" s="65"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="65"/>
+      <c r="I92" s="65"/>
+      <c r="J92" s="65"/>
+      <c r="K92" s="65"/>
+      <c r="L92" s="65"/>
+      <c r="M92" s="65"/>
+      <c r="N92" s="65"/>
+      <c r="O92" s="65"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="45"/>
-      <c r="C93" s="45"/>
-      <c r="D93" s="45"/>
-      <c r="E93" s="45"/>
-      <c r="F93" s="45"/>
-      <c r="G93" s="45"/>
-      <c r="H93" s="45"/>
-      <c r="I93" s="45"/>
-      <c r="J93" s="45"/>
-      <c r="K93" s="45"/>
-      <c r="L93" s="45"/>
-      <c r="M93" s="45"/>
-      <c r="N93" s="45"/>
-      <c r="O93" s="45"/>
+      <c r="B93" s="65"/>
+      <c r="C93" s="65"/>
+      <c r="D93" s="65"/>
+      <c r="E93" s="65"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="65"/>
+      <c r="H93" s="65"/>
+      <c r="I93" s="65"/>
+      <c r="J93" s="65"/>
+      <c r="K93" s="65"/>
+      <c r="L93" s="65"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
+      <c r="O93" s="65"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="45"/>
-      <c r="C94" s="45"/>
-      <c r="D94" s="45"/>
-      <c r="E94" s="45"/>
-      <c r="F94" s="45"/>
-      <c r="G94" s="45"/>
-      <c r="H94" s="45"/>
-      <c r="I94" s="45"/>
-      <c r="J94" s="45"/>
-      <c r="K94" s="45"/>
-      <c r="L94" s="45"/>
-      <c r="M94" s="45"/>
-      <c r="N94" s="45"/>
-      <c r="O94" s="45"/>
+      <c r="B94" s="65"/>
+      <c r="C94" s="65"/>
+      <c r="D94" s="65"/>
+      <c r="E94" s="65"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="65"/>
+      <c r="H94" s="65"/>
+      <c r="I94" s="65"/>
+      <c r="J94" s="65"/>
+      <c r="K94" s="65"/>
+      <c r="L94" s="65"/>
+      <c r="M94" s="65"/>
+      <c r="N94" s="65"/>
+      <c r="O94" s="65"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="45"/>
-      <c r="C95" s="45"/>
-      <c r="D95" s="45"/>
-      <c r="E95" s="45"/>
-      <c r="F95" s="45"/>
-      <c r="G95" s="45"/>
-      <c r="H95" s="45"/>
-      <c r="I95" s="45"/>
-      <c r="J95" s="45"/>
-      <c r="K95" s="45"/>
-      <c r="L95" s="45"/>
-      <c r="M95" s="45"/>
-      <c r="N95" s="45"/>
-      <c r="O95" s="45"/>
+      <c r="B95" s="65"/>
+      <c r="C95" s="65"/>
+      <c r="D95" s="65"/>
+      <c r="E95" s="65"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="65"/>
+      <c r="L95" s="65"/>
+      <c r="M95" s="65"/>
+      <c r="N95" s="65"/>
+      <c r="O95" s="65"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B96" s="45"/>
-      <c r="C96" s="45"/>
-      <c r="D96" s="45"/>
-      <c r="E96" s="45"/>
-      <c r="F96" s="45"/>
-      <c r="G96" s="45"/>
-      <c r="H96" s="45"/>
-      <c r="I96" s="45"/>
-      <c r="J96" s="45"/>
-      <c r="K96" s="45"/>
-      <c r="L96" s="45"/>
-      <c r="M96" s="45"/>
-      <c r="N96" s="45"/>
-      <c r="O96" s="45"/>
+      <c r="B96" s="65"/>
+      <c r="C96" s="65"/>
+      <c r="D96" s="65"/>
+      <c r="E96" s="65"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
+      <c r="J96" s="65"/>
+      <c r="K96" s="65"/>
+      <c r="L96" s="65"/>
+      <c r="M96" s="65"/>
+      <c r="N96" s="65"/>
+      <c r="O96" s="65"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97" s="45"/>
-      <c r="C97" s="45"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="45"/>
-      <c r="J97" s="45"/>
-      <c r="K97" s="45"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="45"/>
-      <c r="N97" s="45"/>
-      <c r="O97" s="45"/>
+      <c r="B97" s="65"/>
+      <c r="C97" s="65"/>
+      <c r="D97" s="65"/>
+      <c r="E97" s="65"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="65"/>
+      <c r="I97" s="65"/>
+      <c r="J97" s="65"/>
+      <c r="K97" s="65"/>
+      <c r="L97" s="65"/>
+      <c r="M97" s="65"/>
+      <c r="N97" s="65"/>
+      <c r="O97" s="65"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="45"/>
-      <c r="C98" s="45"/>
-      <c r="D98" s="45"/>
-      <c r="E98" s="45"/>
-      <c r="F98" s="45"/>
-      <c r="G98" s="45"/>
-      <c r="H98" s="45"/>
-      <c r="I98" s="45"/>
-      <c r="J98" s="45"/>
-      <c r="K98" s="45"/>
-      <c r="L98" s="45"/>
-      <c r="M98" s="45"/>
-      <c r="N98" s="45"/>
-      <c r="O98" s="45"/>
+      <c r="B98" s="65"/>
+      <c r="C98" s="65"/>
+      <c r="D98" s="65"/>
+      <c r="E98" s="65"/>
+      <c r="F98" s="65"/>
+      <c r="G98" s="65"/>
+      <c r="H98" s="65"/>
+      <c r="I98" s="65"/>
+      <c r="J98" s="65"/>
+      <c r="K98" s="65"/>
+      <c r="L98" s="65"/>
+      <c r="M98" s="65"/>
+      <c r="N98" s="65"/>
+      <c r="O98" s="65"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99" s="45"/>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
-      <c r="E99" s="45"/>
-      <c r="F99" s="45"/>
-      <c r="G99" s="45"/>
-      <c r="H99" s="45"/>
-      <c r="I99" s="45"/>
-      <c r="J99" s="45"/>
-      <c r="K99" s="45"/>
-      <c r="L99" s="45"/>
-      <c r="M99" s="45"/>
-      <c r="N99" s="45"/>
-      <c r="O99" s="45"/>
+      <c r="B99" s="65"/>
+      <c r="C99" s="65"/>
+      <c r="D99" s="65"/>
+      <c r="E99" s="65"/>
+      <c r="F99" s="65"/>
+      <c r="G99" s="65"/>
+      <c r="H99" s="65"/>
+      <c r="I99" s="65"/>
+      <c r="J99" s="65"/>
+      <c r="K99" s="65"/>
+      <c r="L99" s="65"/>
+      <c r="M99" s="65"/>
+      <c r="N99" s="65"/>
+      <c r="O99" s="65"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="45"/>
-      <c r="C100" s="45"/>
-      <c r="D100" s="45"/>
-      <c r="E100" s="45"/>
-      <c r="F100" s="45"/>
-      <c r="G100" s="45"/>
-      <c r="H100" s="45"/>
-      <c r="I100" s="45"/>
-      <c r="J100" s="45"/>
-      <c r="K100" s="45"/>
-      <c r="L100" s="45"/>
-      <c r="M100" s="45"/>
-      <c r="N100" s="45"/>
-      <c r="O100" s="45"/>
+      <c r="B100" s="65"/>
+      <c r="C100" s="65"/>
+      <c r="D100" s="65"/>
+      <c r="E100" s="65"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="65"/>
+      <c r="I100" s="65"/>
+      <c r="J100" s="65"/>
+      <c r="K100" s="65"/>
+      <c r="L100" s="65"/>
+      <c r="M100" s="65"/>
+      <c r="N100" s="65"/>
+      <c r="O100" s="65"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="45"/>
-      <c r="C101" s="45"/>
-      <c r="D101" s="45"/>
-      <c r="E101" s="45"/>
-      <c r="F101" s="45"/>
-      <c r="G101" s="45"/>
-      <c r="H101" s="45"/>
-      <c r="I101" s="45"/>
-      <c r="J101" s="45"/>
-      <c r="K101" s="45"/>
-      <c r="L101" s="45"/>
-      <c r="M101" s="45"/>
-      <c r="N101" s="45"/>
-      <c r="O101" s="45"/>
+      <c r="B101" s="65"/>
+      <c r="C101" s="65"/>
+      <c r="D101" s="65"/>
+      <c r="E101" s="65"/>
+      <c r="F101" s="65"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="65"/>
+      <c r="I101" s="65"/>
+      <c r="J101" s="65"/>
+      <c r="K101" s="65"/>
+      <c r="L101" s="65"/>
+      <c r="M101" s="65"/>
+      <c r="N101" s="65"/>
+      <c r="O101" s="65"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B102" s="45"/>
-      <c r="C102" s="45"/>
-      <c r="D102" s="45"/>
-      <c r="E102" s="45"/>
-      <c r="F102" s="45"/>
-      <c r="G102" s="45"/>
-      <c r="H102" s="45"/>
-      <c r="I102" s="45"/>
-      <c r="J102" s="45"/>
-      <c r="K102" s="45"/>
-      <c r="L102" s="45"/>
-      <c r="M102" s="45"/>
-      <c r="N102" s="45"/>
-      <c r="O102" s="45"/>
+      <c r="B102" s="65"/>
+      <c r="C102" s="65"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="65"/>
+      <c r="F102" s="65"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="65"/>
+      <c r="I102" s="65"/>
+      <c r="J102" s="65"/>
+      <c r="K102" s="65"/>
+      <c r="L102" s="65"/>
+      <c r="M102" s="65"/>
+      <c r="N102" s="65"/>
+      <c r="O102" s="65"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B103" s="45"/>
-      <c r="C103" s="45"/>
-      <c r="D103" s="45"/>
-      <c r="E103" s="45"/>
-      <c r="F103" s="45"/>
-      <c r="G103" s="45"/>
-      <c r="H103" s="45"/>
-      <c r="I103" s="45"/>
-      <c r="J103" s="45"/>
-      <c r="K103" s="45"/>
-      <c r="L103" s="45"/>
-      <c r="M103" s="45"/>
-      <c r="N103" s="45"/>
-      <c r="O103" s="45"/>
+      <c r="B103" s="65"/>
+      <c r="C103" s="65"/>
+      <c r="D103" s="65"/>
+      <c r="E103" s="65"/>
+      <c r="F103" s="65"/>
+      <c r="G103" s="65"/>
+      <c r="H103" s="65"/>
+      <c r="I103" s="65"/>
+      <c r="J103" s="65"/>
+      <c r="K103" s="65"/>
+      <c r="L103" s="65"/>
+      <c r="M103" s="65"/>
+      <c r="N103" s="65"/>
+      <c r="O103" s="65"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104" s="45"/>
-      <c r="C104" s="45"/>
-      <c r="D104" s="45"/>
-      <c r="E104" s="45"/>
-      <c r="F104" s="45"/>
-      <c r="G104" s="45"/>
-      <c r="H104" s="45"/>
-      <c r="I104" s="45"/>
-      <c r="J104" s="45"/>
-      <c r="K104" s="45"/>
-      <c r="L104" s="45"/>
-      <c r="M104" s="45"/>
-      <c r="N104" s="45"/>
-      <c r="O104" s="45"/>
+      <c r="B104" s="65"/>
+      <c r="C104" s="65"/>
+      <c r="D104" s="65"/>
+      <c r="E104" s="65"/>
+      <c r="F104" s="65"/>
+      <c r="G104" s="65"/>
+      <c r="H104" s="65"/>
+      <c r="I104" s="65"/>
+      <c r="J104" s="65"/>
+      <c r="K104" s="65"/>
+      <c r="L104" s="65"/>
+      <c r="M104" s="65"/>
+      <c r="N104" s="65"/>
+      <c r="O104" s="65"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105" s="45"/>
-      <c r="C105" s="45"/>
-      <c r="D105" s="45"/>
-      <c r="E105" s="45"/>
-      <c r="F105" s="45"/>
-      <c r="G105" s="45"/>
-      <c r="H105" s="45"/>
-      <c r="I105" s="45"/>
-      <c r="J105" s="45"/>
-      <c r="K105" s="45"/>
-      <c r="L105" s="45"/>
-      <c r="M105" s="45"/>
-      <c r="N105" s="45"/>
-      <c r="O105" s="45"/>
+      <c r="B105" s="65"/>
+      <c r="C105" s="65"/>
+      <c r="D105" s="65"/>
+      <c r="E105" s="65"/>
+      <c r="F105" s="65"/>
+      <c r="G105" s="65"/>
+      <c r="H105" s="65"/>
+      <c r="I105" s="65"/>
+      <c r="J105" s="65"/>
+      <c r="K105" s="65"/>
+      <c r="L105" s="65"/>
+      <c r="M105" s="65"/>
+      <c r="N105" s="65"/>
+      <c r="O105" s="65"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="45"/>
-      <c r="C106" s="45"/>
-      <c r="D106" s="45"/>
-      <c r="E106" s="45"/>
-      <c r="F106" s="45"/>
-      <c r="G106" s="45"/>
-      <c r="H106" s="45"/>
-      <c r="I106" s="45"/>
-      <c r="J106" s="45"/>
-      <c r="K106" s="45"/>
-      <c r="L106" s="45"/>
-      <c r="M106" s="45"/>
-      <c r="N106" s="45"/>
-      <c r="O106" s="45"/>
+      <c r="B106" s="65"/>
+      <c r="C106" s="65"/>
+      <c r="D106" s="65"/>
+      <c r="E106" s="65"/>
+      <c r="F106" s="65"/>
+      <c r="G106" s="65"/>
+      <c r="H106" s="65"/>
+      <c r="I106" s="65"/>
+      <c r="J106" s="65"/>
+      <c r="K106" s="65"/>
+      <c r="L106" s="65"/>
+      <c r="M106" s="65"/>
+      <c r="N106" s="65"/>
+      <c r="O106" s="65"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="45"/>
-      <c r="C107" s="45"/>
-      <c r="D107" s="45"/>
-      <c r="E107" s="45"/>
-      <c r="F107" s="45"/>
-      <c r="G107" s="45"/>
-      <c r="H107" s="45"/>
-      <c r="I107" s="45"/>
-      <c r="J107" s="45"/>
-      <c r="K107" s="45"/>
-      <c r="L107" s="45"/>
-      <c r="M107" s="45"/>
-      <c r="N107" s="45"/>
-      <c r="O107" s="45"/>
+      <c r="B107" s="65"/>
+      <c r="C107" s="65"/>
+      <c r="D107" s="65"/>
+      <c r="E107" s="65"/>
+      <c r="F107" s="65"/>
+      <c r="G107" s="65"/>
+      <c r="H107" s="65"/>
+      <c r="I107" s="65"/>
+      <c r="J107" s="65"/>
+      <c r="K107" s="65"/>
+      <c r="L107" s="65"/>
+      <c r="M107" s="65"/>
+      <c r="N107" s="65"/>
+      <c r="O107" s="65"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="45"/>
-      <c r="C108" s="45"/>
-      <c r="D108" s="45"/>
-      <c r="E108" s="45"/>
-      <c r="F108" s="45"/>
-      <c r="G108" s="45"/>
-      <c r="H108" s="45"/>
-      <c r="I108" s="45"/>
-      <c r="J108" s="45"/>
-      <c r="K108" s="45"/>
-      <c r="L108" s="45"/>
-      <c r="M108" s="45"/>
-      <c r="N108" s="45"/>
-      <c r="O108" s="45"/>
+      <c r="B108" s="65"/>
+      <c r="C108" s="65"/>
+      <c r="D108" s="65"/>
+      <c r="E108" s="65"/>
+      <c r="F108" s="65"/>
+      <c r="G108" s="65"/>
+      <c r="H108" s="65"/>
+      <c r="I108" s="65"/>
+      <c r="J108" s="65"/>
+      <c r="K108" s="65"/>
+      <c r="L108" s="65"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="65"/>
+      <c r="O108" s="65"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="45"/>
-      <c r="C109" s="45"/>
-      <c r="D109" s="45"/>
-      <c r="E109" s="45"/>
-      <c r="F109" s="45"/>
-      <c r="G109" s="45"/>
-      <c r="H109" s="45"/>
-      <c r="I109" s="45"/>
-      <c r="J109" s="45"/>
-      <c r="K109" s="45"/>
-      <c r="L109" s="45"/>
-      <c r="M109" s="45"/>
-      <c r="N109" s="45"/>
-      <c r="O109" s="45"/>
+      <c r="B109" s="65"/>
+      <c r="C109" s="65"/>
+      <c r="D109" s="65"/>
+      <c r="E109" s="65"/>
+      <c r="F109" s="65"/>
+      <c r="G109" s="65"/>
+      <c r="H109" s="65"/>
+      <c r="I109" s="65"/>
+      <c r="J109" s="65"/>
+      <c r="K109" s="65"/>
+      <c r="L109" s="65"/>
+      <c r="M109" s="65"/>
+      <c r="N109" s="65"/>
+      <c r="O109" s="65"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B110" s="45"/>
-      <c r="C110" s="45"/>
-      <c r="D110" s="45"/>
-      <c r="E110" s="45"/>
-      <c r="F110" s="45"/>
-      <c r="G110" s="45"/>
-      <c r="H110" s="45"/>
-      <c r="I110" s="45"/>
-      <c r="J110" s="45"/>
-      <c r="K110" s="45"/>
-      <c r="L110" s="45"/>
-      <c r="M110" s="45"/>
-      <c r="N110" s="45"/>
-      <c r="O110" s="45"/>
+      <c r="B110" s="65"/>
+      <c r="C110" s="65"/>
+      <c r="D110" s="65"/>
+      <c r="E110" s="65"/>
+      <c r="F110" s="65"/>
+      <c r="G110" s="65"/>
+      <c r="H110" s="65"/>
+      <c r="I110" s="65"/>
+      <c r="J110" s="65"/>
+      <c r="K110" s="65"/>
+      <c r="L110" s="65"/>
+      <c r="M110" s="65"/>
+      <c r="N110" s="65"/>
+      <c r="O110" s="65"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B111" s="45"/>
-      <c r="C111" s="45"/>
-      <c r="D111" s="45"/>
-      <c r="E111" s="45"/>
-      <c r="F111" s="45"/>
-      <c r="G111" s="45"/>
-      <c r="H111" s="45"/>
-      <c r="I111" s="45"/>
-      <c r="J111" s="45"/>
-      <c r="K111" s="45"/>
-      <c r="L111" s="45"/>
-      <c r="M111" s="45"/>
-      <c r="N111" s="45"/>
-      <c r="O111" s="45"/>
+      <c r="B111" s="65"/>
+      <c r="C111" s="65"/>
+      <c r="D111" s="65"/>
+      <c r="E111" s="65"/>
+      <c r="F111" s="65"/>
+      <c r="G111" s="65"/>
+      <c r="H111" s="65"/>
+      <c r="I111" s="65"/>
+      <c r="J111" s="65"/>
+      <c r="K111" s="65"/>
+      <c r="L111" s="65"/>
+      <c r="M111" s="65"/>
+      <c r="N111" s="65"/>
+      <c r="O111" s="65"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="45"/>
-      <c r="C112" s="45"/>
-      <c r="D112" s="45"/>
-      <c r="E112" s="45"/>
-      <c r="F112" s="45"/>
-      <c r="G112" s="45"/>
-      <c r="H112" s="45"/>
-      <c r="I112" s="45"/>
-      <c r="J112" s="45"/>
-      <c r="K112" s="45"/>
-      <c r="L112" s="45"/>
-      <c r="M112" s="45"/>
-      <c r="N112" s="45"/>
-      <c r="O112" s="45"/>
+      <c r="B112" s="65"/>
+      <c r="C112" s="65"/>
+      <c r="D112" s="65"/>
+      <c r="E112" s="65"/>
+      <c r="F112" s="65"/>
+      <c r="G112" s="65"/>
+      <c r="H112" s="65"/>
+      <c r="I112" s="65"/>
+      <c r="J112" s="65"/>
+      <c r="K112" s="65"/>
+      <c r="L112" s="65"/>
+      <c r="M112" s="65"/>
+      <c r="N112" s="65"/>
+      <c r="O112" s="65"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="45"/>
-      <c r="C113" s="45"/>
-      <c r="D113" s="45"/>
-      <c r="E113" s="45"/>
-      <c r="F113" s="45"/>
-      <c r="G113" s="45"/>
-      <c r="H113" s="45"/>
-      <c r="I113" s="45"/>
-      <c r="J113" s="45"/>
-      <c r="K113" s="45"/>
-      <c r="L113" s="45"/>
-      <c r="M113" s="45"/>
-      <c r="N113" s="45"/>
-      <c r="O113" s="45"/>
+      <c r="B113" s="65"/>
+      <c r="C113" s="65"/>
+      <c r="D113" s="65"/>
+      <c r="E113" s="65"/>
+      <c r="F113" s="65"/>
+      <c r="G113" s="65"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65"/>
+      <c r="J113" s="65"/>
+      <c r="K113" s="65"/>
+      <c r="L113" s="65"/>
+      <c r="M113" s="65"/>
+      <c r="N113" s="65"/>
+      <c r="O113" s="65"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="45"/>
-      <c r="C114" s="45"/>
-      <c r="D114" s="45"/>
-      <c r="E114" s="45"/>
-      <c r="F114" s="45"/>
-      <c r="G114" s="45"/>
-      <c r="H114" s="45"/>
-      <c r="I114" s="45"/>
-      <c r="J114" s="45"/>
-      <c r="K114" s="45"/>
-      <c r="L114" s="45"/>
-      <c r="M114" s="45"/>
-      <c r="N114" s="45"/>
-      <c r="O114" s="45"/>
+      <c r="B114" s="65"/>
+      <c r="C114" s="65"/>
+      <c r="D114" s="65"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="65"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65"/>
+      <c r="J114" s="65"/>
+      <c r="K114" s="65"/>
+      <c r="L114" s="65"/>
+      <c r="M114" s="65"/>
+      <c r="N114" s="65"/>
+      <c r="O114" s="65"/>
     </row>
     <row r="115" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="45"/>
-      <c r="C115" s="45"/>
-      <c r="D115" s="45"/>
-      <c r="E115" s="45"/>
-      <c r="F115" s="45"/>
-      <c r="G115" s="45"/>
-      <c r="H115" s="45"/>
-      <c r="I115" s="45"/>
-      <c r="J115" s="45"/>
-      <c r="K115" s="45"/>
-      <c r="L115" s="45"/>
-      <c r="M115" s="45"/>
-      <c r="N115" s="45"/>
-      <c r="O115" s="45"/>
+      <c r="B115" s="65"/>
+      <c r="C115" s="65"/>
+      <c r="D115" s="65"/>
+      <c r="E115" s="65"/>
+      <c r="F115" s="65"/>
+      <c r="G115" s="65"/>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65"/>
+      <c r="J115" s="65"/>
+      <c r="K115" s="65"/>
+      <c r="L115" s="65"/>
+      <c r="M115" s="65"/>
+      <c r="N115" s="65"/>
+      <c r="O115" s="65"/>
     </row>
     <row r="116" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="40"/>
@@ -4578,45 +4538,63 @@
     </row>
     <row r="117" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="46" t="s">
+      <c r="B118" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="C118" s="46"/>
-      <c r="D118" s="46"/>
-      <c r="E118" s="46"/>
-      <c r="F118" s="46"/>
-      <c r="G118" s="46"/>
-      <c r="H118" s="46"/>
-      <c r="I118" s="46"/>
-      <c r="J118" s="46"/>
-      <c r="K118" s="46"/>
-      <c r="L118" s="46"/>
-      <c r="M118" s="46"/>
-      <c r="N118" s="46"/>
-      <c r="O118" s="46"/>
+      <c r="C118" s="66"/>
+      <c r="D118" s="66"/>
+      <c r="E118" s="66"/>
+      <c r="F118" s="66"/>
+      <c r="G118" s="66"/>
+      <c r="H118" s="66"/>
+      <c r="I118" s="66"/>
+      <c r="J118" s="66"/>
+      <c r="K118" s="66"/>
+      <c r="L118" s="66"/>
+      <c r="M118" s="66"/>
+      <c r="N118" s="66"/>
+      <c r="O118" s="66"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="46"/>
-      <c r="C119" s="46"/>
-      <c r="D119" s="46"/>
-      <c r="E119" s="46"/>
-      <c r="F119" s="46"/>
-      <c r="G119" s="46"/>
-      <c r="H119" s="46"/>
-      <c r="I119" s="46"/>
-      <c r="J119" s="46"/>
-      <c r="K119" s="46"/>
-      <c r="L119" s="46"/>
-      <c r="M119" s="46"/>
-      <c r="N119" s="46"/>
-      <c r="O119" s="46"/>
+      <c r="B119" s="66"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="66"/>
+      <c r="H119" s="66"/>
+      <c r="I119" s="66"/>
+      <c r="J119" s="66"/>
+      <c r="K119" s="66"/>
+      <c r="L119" s="66"/>
+      <c r="M119" s="66"/>
+      <c r="N119" s="66"/>
+      <c r="O119" s="66"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
+    <mergeCell ref="B72:H115"/>
+    <mergeCell ref="I72:O115"/>
+    <mergeCell ref="B118:O119"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="B70:O70"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="I38:O38"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="B42:O42"/>
+    <mergeCell ref="F45:G45"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="A6:O6"/>
     <mergeCell ref="B17:O17"/>
@@ -4633,23 +4611,6 @@
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="H14:L14"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="B42:O42"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B72:H115"/>
-    <mergeCell ref="I72:O115"/>
-    <mergeCell ref="B118:O119"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="B70:O70"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="L53:O53"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add dropdown menu for selecting superintendent signature type in leave application downloads
Added optional signatureChoice parameter to leave application download route and controller to allow users to select between Assistant School Division Superintendent and Schools Division Superintendent signatures. Implemented dropdown menu in teacher and non-teaching dashboards with Alpine.js for signature selection. Updated DLAppForLeaveController to populate Administrative Officer VI, School Head, and Division Superintendent signatures from
</commit_message>
<xml_diff>
--- a/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
+++ b/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source Codes\personal-info-management-system\resources\views\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96994F0-B4CA-4F76-BAF5-9BA6C9F384E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A3FC61-4028-4DB7-B34B-B537D6D69A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Civil Service Form No. 6</t>
   </si>
@@ -568,9 +568,6 @@
   </si>
   <si>
     <t>7.C APPROVED FOR:</t>
-  </si>
-  <si>
-    <t>7. D   DISAPPROVED DUE TO:</t>
   </si>
   <si>
     <t>days with pay</t>
@@ -934,15 +931,6 @@
     <t>Feverish and Headache</t>
   </si>
   <si>
-    <t>JULIUS CESAR L. DE LA CERNA</t>
-  </si>
-  <si>
-    <t>JOSEMILO P. RUIZ EdD, CESE</t>
-  </si>
-  <si>
-    <t>Assistant School Division Superintendent</t>
-  </si>
-  <si>
     <t>Region VIII (Eastern Visayas)</t>
   </si>
   <si>
@@ -952,10 +940,13 @@
     <t>Diversion Road, Brgy. Ga-as, Baybay City, Leyte</t>
   </si>
   <si>
-    <t>AO IV / HRMO II</t>
-  </si>
-  <si>
     <t>SCHOOL HEAD/CLUSTER IN-CHARGE</t>
+  </si>
+  <si>
+    <t>7.  DISAPPROVED DUE TO:</t>
+  </si>
+  <si>
+    <t>ADMINISTRATIVE OFFICER VI (HRMO II)</t>
   </si>
 </sst>
 </file>
@@ -1399,6 +1390,87 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1408,15 +1480,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1439,78 +1502,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1883,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27B6FB-8E85-4B80-9281-508316E41DF7}">
   <dimension ref="A1:WVX123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62:L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2932,121 +2923,121 @@
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
+      <c r="A6" s="72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
+      <c r="A7" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
+      <c r="A8" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
     </row>
     <row r="9" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -3058,38 +3049,38 @@
       <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52" t="s">
+      <c r="H11" s="76"/>
+      <c r="I11" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52" t="s">
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="53"/>
+      <c r="O11" s="77"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
+      <c r="C12" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="80"/>
     </row>
     <row r="13" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
@@ -3118,11 +3109,11 @@
       <c r="G14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
       <c r="M14" s="14"/>
       <c r="N14" s="6" t="s">
         <v>13</v>
@@ -3147,22 +3138,22 @@
     </row>
     <row r="16" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="48"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="68"/>
     </row>
     <row r="18" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
@@ -3276,10 +3267,10 @@
         <v>28</v>
       </c>
       <c r="M25" s="21"/>
-      <c r="N25" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="O25" s="44"/>
+      <c r="N25" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="O25" s="71"/>
     </row>
     <row r="26" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
@@ -3388,8 +3379,8 @@
       <c r="E33" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="22"/>
       <c r="I33" s="8"/>
       <c r="J33" s="20"/>
@@ -3437,9 +3428,9 @@
     </row>
     <row r="36" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="22"/>
       <c r="I36" s="8"/>
       <c r="J36" s="20"/>
@@ -3465,32 +3456,32 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
-      <c r="E38" s="58">
+      <c r="E38" s="61">
         <v>45330</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="80"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="59"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="60" t="s">
+      <c r="I39" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="62"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="65"/>
     </row>
     <row r="40" spans="2:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
@@ -3510,22 +3501,22 @@
     </row>
     <row r="41" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="47"/>
-      <c r="M42" s="47"/>
-      <c r="N42" s="47"/>
-      <c r="O42" s="48"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="68"/>
     </row>
     <row r="43" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -3553,8 +3544,8 @@
       <c r="E45" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="21"/>
       <c r="I45" s="8"/>
       <c r="O45" s="22"/>
@@ -3643,33 +3634,31 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="E53" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
       <c r="I53" s="8"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="76"/>
-      <c r="O53" s="77"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="56"/>
     </row>
     <row r="54" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
-      <c r="E54" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
+      <c r="E54" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
       <c r="I54" s="38"/>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
-      <c r="L54" s="68" t="s">
-        <v>80</v>
-      </c>
-      <c r="M54" s="68"/>
-      <c r="N54" s="68"/>
-      <c r="O54" s="69"/>
+      <c r="L54" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="48"/>
     </row>
     <row r="55" spans="2:15" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
@@ -3698,21 +3687,20 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
-      <c r="L56" s="7"/>
       <c r="M56" s="7"/>
       <c r="N56" s="26"/>
       <c r="O56" s="27"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="70"/>
-      <c r="C57" s="71"/>
-      <c r="D57" s="71"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L57" s="10"/>
       <c r="M57" s="10"/>
@@ -3724,7 +3712,7 @@
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
       <c r="E58" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L58" s="10"/>
       <c r="M58" s="37"/>
@@ -3736,7 +3724,7 @@
       <c r="C59" s="26"/>
       <c r="D59" s="26"/>
       <c r="E59" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L59" s="10"/>
       <c r="M59" s="10"/>
@@ -3749,26 +3737,22 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
-      <c r="G61" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="H61" s="71"/>
-      <c r="I61" s="71"/>
-      <c r="J61" s="71"/>
-      <c r="K61" s="71"/>
-      <c r="L61" s="71"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="50"/>
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
-      <c r="G62" s="72" t="s">
-        <v>75</v>
-      </c>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3794,731 +3778,731 @@
     <row r="68" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74"/>
-      <c r="L70" s="74"/>
-      <c r="M70" s="74"/>
-      <c r="N70" s="74"/>
-      <c r="O70" s="75"/>
+      <c r="B70" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="53"/>
+      <c r="L70" s="53"/>
+      <c r="M70" s="53"/>
+      <c r="N70" s="53"/>
+      <c r="O70" s="54"/>
     </row>
     <row r="71" spans="2:15" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="64" t="s">
+      <c r="B72" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
-      <c r="I72" s="64" t="s">
-        <v>69</v>
-      </c>
-      <c r="J72" s="65"/>
-      <c r="K72" s="65"/>
-      <c r="L72" s="65"/>
-      <c r="M72" s="65"/>
-      <c r="N72" s="65"/>
-      <c r="O72" s="65"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44"/>
+      <c r="N72" s="44"/>
+      <c r="O72" s="44"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
-      <c r="K73" s="65"/>
-      <c r="L73" s="65"/>
-      <c r="M73" s="65"/>
-      <c r="N73" s="65"/>
-      <c r="O73" s="65"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="44"/>
+      <c r="M73" s="44"/>
+      <c r="N73" s="44"/>
+      <c r="O73" s="44"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="65"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
-      <c r="K74" s="65"/>
-      <c r="L74" s="65"/>
-      <c r="M74" s="65"/>
-      <c r="N74" s="65"/>
-      <c r="O74" s="65"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="65"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="65"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="65"/>
-      <c r="H75" s="65"/>
-      <c r="I75" s="65"/>
-      <c r="J75" s="65"/>
-      <c r="K75" s="65"/>
-      <c r="L75" s="65"/>
-      <c r="M75" s="65"/>
-      <c r="N75" s="65"/>
-      <c r="O75" s="65"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="44"/>
+      <c r="J75" s="44"/>
+      <c r="K75" s="44"/>
+      <c r="L75" s="44"/>
+      <c r="M75" s="44"/>
+      <c r="N75" s="44"/>
+      <c r="O75" s="44"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="65"/>
-      <c r="C76" s="65"/>
-      <c r="D76" s="65"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="65"/>
-      <c r="G76" s="65"/>
-      <c r="H76" s="65"/>
-      <c r="I76" s="65"/>
-      <c r="J76" s="65"/>
-      <c r="K76" s="65"/>
-      <c r="L76" s="65"/>
-      <c r="M76" s="65"/>
-      <c r="N76" s="65"/>
-      <c r="O76" s="65"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="44"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="44"/>
+      <c r="O76" s="44"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="65"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="65"/>
-      <c r="E77" s="65"/>
-      <c r="F77" s="65"/>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="65"/>
-      <c r="J77" s="65"/>
-      <c r="K77" s="65"/>
-      <c r="L77" s="65"/>
-      <c r="M77" s="65"/>
-      <c r="N77" s="65"/>
-      <c r="O77" s="65"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="44"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="44"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="44"/>
+      <c r="O77" s="44"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="65"/>
-      <c r="C78" s="65"/>
-      <c r="D78" s="65"/>
-      <c r="E78" s="65"/>
-      <c r="F78" s="65"/>
-      <c r="G78" s="65"/>
-      <c r="H78" s="65"/>
-      <c r="I78" s="65"/>
-      <c r="J78" s="65"/>
-      <c r="K78" s="65"/>
-      <c r="L78" s="65"/>
-      <c r="M78" s="65"/>
-      <c r="N78" s="65"/>
-      <c r="O78" s="65"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="44"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44"/>
+      <c r="N78" s="44"/>
+      <c r="O78" s="44"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="65"/>
-      <c r="C79" s="65"/>
-      <c r="D79" s="65"/>
-      <c r="E79" s="65"/>
-      <c r="F79" s="65"/>
-      <c r="G79" s="65"/>
-      <c r="H79" s="65"/>
-      <c r="I79" s="65"/>
-      <c r="J79" s="65"/>
-      <c r="K79" s="65"/>
-      <c r="L79" s="65"/>
-      <c r="M79" s="65"/>
-      <c r="N79" s="65"/>
-      <c r="O79" s="65"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
+      <c r="I79" s="44"/>
+      <c r="J79" s="44"/>
+      <c r="K79" s="44"/>
+      <c r="L79" s="44"/>
+      <c r="M79" s="44"/>
+      <c r="N79" s="44"/>
+      <c r="O79" s="44"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="65"/>
-      <c r="C80" s="65"/>
-      <c r="D80" s="65"/>
-      <c r="E80" s="65"/>
-      <c r="F80" s="65"/>
-      <c r="G80" s="65"/>
-      <c r="H80" s="65"/>
-      <c r="I80" s="65"/>
-      <c r="J80" s="65"/>
-      <c r="K80" s="65"/>
-      <c r="L80" s="65"/>
-      <c r="M80" s="65"/>
-      <c r="N80" s="65"/>
-      <c r="O80" s="65"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="44"/>
+      <c r="M80" s="44"/>
+      <c r="N80" s="44"/>
+      <c r="O80" s="44"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="65"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="65"/>
-      <c r="E81" s="65"/>
-      <c r="F81" s="65"/>
-      <c r="G81" s="65"/>
-      <c r="H81" s="65"/>
-      <c r="I81" s="65"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="65"/>
-      <c r="L81" s="65"/>
-      <c r="M81" s="65"/>
-      <c r="N81" s="65"/>
-      <c r="O81" s="65"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="44"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
+      <c r="M81" s="44"/>
+      <c r="N81" s="44"/>
+      <c r="O81" s="44"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="65"/>
-      <c r="E82" s="65"/>
-      <c r="F82" s="65"/>
-      <c r="G82" s="65"/>
-      <c r="H82" s="65"/>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
-      <c r="M82" s="65"/>
-      <c r="N82" s="65"/>
-      <c r="O82" s="65"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="44"/>
+      <c r="K82" s="44"/>
+      <c r="L82" s="44"/>
+      <c r="M82" s="44"/>
+      <c r="N82" s="44"/>
+      <c r="O82" s="44"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="65"/>
-      <c r="C83" s="65"/>
-      <c r="D83" s="65"/>
-      <c r="E83" s="65"/>
-      <c r="F83" s="65"/>
-      <c r="G83" s="65"/>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="65"/>
-      <c r="M83" s="65"/>
-      <c r="N83" s="65"/>
-      <c r="O83" s="65"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="44"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="44"/>
+      <c r="O83" s="44"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="65"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="65"/>
-      <c r="G84" s="65"/>
-      <c r="H84" s="65"/>
-      <c r="I84" s="65"/>
-      <c r="J84" s="65"/>
-      <c r="K84" s="65"/>
-      <c r="L84" s="65"/>
-      <c r="M84" s="65"/>
-      <c r="N84" s="65"/>
-      <c r="O84" s="65"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="44"/>
+      <c r="K84" s="44"/>
+      <c r="L84" s="44"/>
+      <c r="M84" s="44"/>
+      <c r="N84" s="44"/>
+      <c r="O84" s="44"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="65"/>
-      <c r="C85" s="65"/>
-      <c r="D85" s="65"/>
-      <c r="E85" s="65"/>
-      <c r="F85" s="65"/>
-      <c r="G85" s="65"/>
-      <c r="H85" s="65"/>
-      <c r="I85" s="65"/>
-      <c r="J85" s="65"/>
-      <c r="K85" s="65"/>
-      <c r="L85" s="65"/>
-      <c r="M85" s="65"/>
-      <c r="N85" s="65"/>
-      <c r="O85" s="65"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="44"/>
+      <c r="M85" s="44"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="44"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="65"/>
-      <c r="C86" s="65"/>
-      <c r="D86" s="65"/>
-      <c r="E86" s="65"/>
-      <c r="F86" s="65"/>
-      <c r="G86" s="65"/>
-      <c r="H86" s="65"/>
-      <c r="I86" s="65"/>
-      <c r="J86" s="65"/>
-      <c r="K86" s="65"/>
-      <c r="L86" s="65"/>
-      <c r="M86" s="65"/>
-      <c r="N86" s="65"/>
-      <c r="O86" s="65"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="44"/>
+      <c r="J86" s="44"/>
+      <c r="K86" s="44"/>
+      <c r="L86" s="44"/>
+      <c r="M86" s="44"/>
+      <c r="N86" s="44"/>
+      <c r="O86" s="44"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="65"/>
-      <c r="C87" s="65"/>
-      <c r="D87" s="65"/>
-      <c r="E87" s="65"/>
-      <c r="F87" s="65"/>
-      <c r="G87" s="65"/>
-      <c r="H87" s="65"/>
-      <c r="I87" s="65"/>
-      <c r="J87" s="65"/>
-      <c r="K87" s="65"/>
-      <c r="L87" s="65"/>
-      <c r="M87" s="65"/>
-      <c r="N87" s="65"/>
-      <c r="O87" s="65"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="44"/>
+      <c r="K87" s="44"/>
+      <c r="L87" s="44"/>
+      <c r="M87" s="44"/>
+      <c r="N87" s="44"/>
+      <c r="O87" s="44"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="65"/>
-      <c r="C88" s="65"/>
-      <c r="D88" s="65"/>
-      <c r="E88" s="65"/>
-      <c r="F88" s="65"/>
-      <c r="G88" s="65"/>
-      <c r="H88" s="65"/>
-      <c r="I88" s="65"/>
-      <c r="J88" s="65"/>
-      <c r="K88" s="65"/>
-      <c r="L88" s="65"/>
-      <c r="M88" s="65"/>
-      <c r="N88" s="65"/>
-      <c r="O88" s="65"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="44"/>
+      <c r="J88" s="44"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="44"/>
+      <c r="M88" s="44"/>
+      <c r="N88" s="44"/>
+      <c r="O88" s="44"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="65"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="65"/>
-      <c r="E89" s="65"/>
-      <c r="F89" s="65"/>
-      <c r="G89" s="65"/>
-      <c r="H89" s="65"/>
-      <c r="I89" s="65"/>
-      <c r="J89" s="65"/>
-      <c r="K89" s="65"/>
-      <c r="L89" s="65"/>
-      <c r="M89" s="65"/>
-      <c r="N89" s="65"/>
-      <c r="O89" s="65"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="44"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="44"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="44"/>
+      <c r="M89" s="44"/>
+      <c r="N89" s="44"/>
+      <c r="O89" s="44"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="65"/>
-      <c r="C90" s="65"/>
-      <c r="D90" s="65"/>
-      <c r="E90" s="65"/>
-      <c r="F90" s="65"/>
-      <c r="G90" s="65"/>
-      <c r="H90" s="65"/>
-      <c r="I90" s="65"/>
-      <c r="J90" s="65"/>
-      <c r="K90" s="65"/>
-      <c r="L90" s="65"/>
-      <c r="M90" s="65"/>
-      <c r="N90" s="65"/>
-      <c r="O90" s="65"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="44"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="44"/>
+      <c r="M90" s="44"/>
+      <c r="N90" s="44"/>
+      <c r="O90" s="44"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="65"/>
-      <c r="C91" s="65"/>
-      <c r="D91" s="65"/>
-      <c r="E91" s="65"/>
-      <c r="F91" s="65"/>
-      <c r="G91" s="65"/>
-      <c r="H91" s="65"/>
-      <c r="I91" s="65"/>
-      <c r="J91" s="65"/>
-      <c r="K91" s="65"/>
-      <c r="L91" s="65"/>
-      <c r="M91" s="65"/>
-      <c r="N91" s="65"/>
-      <c r="O91" s="65"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="44"/>
+      <c r="I91" s="44"/>
+      <c r="J91" s="44"/>
+      <c r="K91" s="44"/>
+      <c r="L91" s="44"/>
+      <c r="M91" s="44"/>
+      <c r="N91" s="44"/>
+      <c r="O91" s="44"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="65"/>
-      <c r="C92" s="65"/>
-      <c r="D92" s="65"/>
-      <c r="E92" s="65"/>
-      <c r="F92" s="65"/>
-      <c r="G92" s="65"/>
-      <c r="H92" s="65"/>
-      <c r="I92" s="65"/>
-      <c r="J92" s="65"/>
-      <c r="K92" s="65"/>
-      <c r="L92" s="65"/>
-      <c r="M92" s="65"/>
-      <c r="N92" s="65"/>
-      <c r="O92" s="65"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="44"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="44"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="44"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="44"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="65"/>
-      <c r="C93" s="65"/>
-      <c r="D93" s="65"/>
-      <c r="E93" s="65"/>
-      <c r="F93" s="65"/>
-      <c r="G93" s="65"/>
-      <c r="H93" s="65"/>
-      <c r="I93" s="65"/>
-      <c r="J93" s="65"/>
-      <c r="K93" s="65"/>
-      <c r="L93" s="65"/>
-      <c r="M93" s="65"/>
-      <c r="N93" s="65"/>
-      <c r="O93" s="65"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="44"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="44"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="44"/>
+      <c r="O93" s="44"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="65"/>
-      <c r="C94" s="65"/>
-      <c r="D94" s="65"/>
-      <c r="E94" s="65"/>
-      <c r="F94" s="65"/>
-      <c r="G94" s="65"/>
-      <c r="H94" s="65"/>
-      <c r="I94" s="65"/>
-      <c r="J94" s="65"/>
-      <c r="K94" s="65"/>
-      <c r="L94" s="65"/>
-      <c r="M94" s="65"/>
-      <c r="N94" s="65"/>
-      <c r="O94" s="65"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="44"/>
+      <c r="I94" s="44"/>
+      <c r="J94" s="44"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="44"/>
+      <c r="M94" s="44"/>
+      <c r="N94" s="44"/>
+      <c r="O94" s="44"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="65"/>
-      <c r="C95" s="65"/>
-      <c r="D95" s="65"/>
-      <c r="E95" s="65"/>
-      <c r="F95" s="65"/>
-      <c r="G95" s="65"/>
-      <c r="H95" s="65"/>
-      <c r="I95" s="65"/>
-      <c r="J95" s="65"/>
-      <c r="K95" s="65"/>
-      <c r="L95" s="65"/>
-      <c r="M95" s="65"/>
-      <c r="N95" s="65"/>
-      <c r="O95" s="65"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="44"/>
+      <c r="I95" s="44"/>
+      <c r="J95" s="44"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="44"/>
+      <c r="M95" s="44"/>
+      <c r="N95" s="44"/>
+      <c r="O95" s="44"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B96" s="65"/>
-      <c r="C96" s="65"/>
-      <c r="D96" s="65"/>
-      <c r="E96" s="65"/>
-      <c r="F96" s="65"/>
-      <c r="G96" s="65"/>
-      <c r="H96" s="65"/>
-      <c r="I96" s="65"/>
-      <c r="J96" s="65"/>
-      <c r="K96" s="65"/>
-      <c r="L96" s="65"/>
-      <c r="M96" s="65"/>
-      <c r="N96" s="65"/>
-      <c r="O96" s="65"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+      <c r="I96" s="44"/>
+      <c r="J96" s="44"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="44"/>
+      <c r="M96" s="44"/>
+      <c r="N96" s="44"/>
+      <c r="O96" s="44"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97" s="65"/>
-      <c r="C97" s="65"/>
-      <c r="D97" s="65"/>
-      <c r="E97" s="65"/>
-      <c r="F97" s="65"/>
-      <c r="G97" s="65"/>
-      <c r="H97" s="65"/>
-      <c r="I97" s="65"/>
-      <c r="J97" s="65"/>
-      <c r="K97" s="65"/>
-      <c r="L97" s="65"/>
-      <c r="M97" s="65"/>
-      <c r="N97" s="65"/>
-      <c r="O97" s="65"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44"/>
+      <c r="J97" s="44"/>
+      <c r="K97" s="44"/>
+      <c r="L97" s="44"/>
+      <c r="M97" s="44"/>
+      <c r="N97" s="44"/>
+      <c r="O97" s="44"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="65"/>
-      <c r="C98" s="65"/>
-      <c r="D98" s="65"/>
-      <c r="E98" s="65"/>
-      <c r="F98" s="65"/>
-      <c r="G98" s="65"/>
-      <c r="H98" s="65"/>
-      <c r="I98" s="65"/>
-      <c r="J98" s="65"/>
-      <c r="K98" s="65"/>
-      <c r="L98" s="65"/>
-      <c r="M98" s="65"/>
-      <c r="N98" s="65"/>
-      <c r="O98" s="65"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="44"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="44"/>
+      <c r="M98" s="44"/>
+      <c r="N98" s="44"/>
+      <c r="O98" s="44"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99" s="65"/>
-      <c r="C99" s="65"/>
-      <c r="D99" s="65"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="65"/>
-      <c r="G99" s="65"/>
-      <c r="H99" s="65"/>
-      <c r="I99" s="65"/>
-      <c r="J99" s="65"/>
-      <c r="K99" s="65"/>
-      <c r="L99" s="65"/>
-      <c r="M99" s="65"/>
-      <c r="N99" s="65"/>
-      <c r="O99" s="65"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+      <c r="I99" s="44"/>
+      <c r="J99" s="44"/>
+      <c r="K99" s="44"/>
+      <c r="L99" s="44"/>
+      <c r="M99" s="44"/>
+      <c r="N99" s="44"/>
+      <c r="O99" s="44"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="65"/>
-      <c r="C100" s="65"/>
-      <c r="D100" s="65"/>
-      <c r="E100" s="65"/>
-      <c r="F100" s="65"/>
-      <c r="G100" s="65"/>
-      <c r="H100" s="65"/>
-      <c r="I100" s="65"/>
-      <c r="J100" s="65"/>
-      <c r="K100" s="65"/>
-      <c r="L100" s="65"/>
-      <c r="M100" s="65"/>
-      <c r="N100" s="65"/>
-      <c r="O100" s="65"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+      <c r="I100" s="44"/>
+      <c r="J100" s="44"/>
+      <c r="K100" s="44"/>
+      <c r="L100" s="44"/>
+      <c r="M100" s="44"/>
+      <c r="N100" s="44"/>
+      <c r="O100" s="44"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="65"/>
-      <c r="C101" s="65"/>
-      <c r="D101" s="65"/>
-      <c r="E101" s="65"/>
-      <c r="F101" s="65"/>
-      <c r="G101" s="65"/>
-      <c r="H101" s="65"/>
-      <c r="I101" s="65"/>
-      <c r="J101" s="65"/>
-      <c r="K101" s="65"/>
-      <c r="L101" s="65"/>
-      <c r="M101" s="65"/>
-      <c r="N101" s="65"/>
-      <c r="O101" s="65"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="44"/>
+      <c r="E101" s="44"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="44"/>
+      <c r="I101" s="44"/>
+      <c r="J101" s="44"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="44"/>
+      <c r="M101" s="44"/>
+      <c r="N101" s="44"/>
+      <c r="O101" s="44"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B102" s="65"/>
-      <c r="C102" s="65"/>
-      <c r="D102" s="65"/>
-      <c r="E102" s="65"/>
-      <c r="F102" s="65"/>
-      <c r="G102" s="65"/>
-      <c r="H102" s="65"/>
-      <c r="I102" s="65"/>
-      <c r="J102" s="65"/>
-      <c r="K102" s="65"/>
-      <c r="L102" s="65"/>
-      <c r="M102" s="65"/>
-      <c r="N102" s="65"/>
-      <c r="O102" s="65"/>
+      <c r="B102" s="44"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="44"/>
+      <c r="I102" s="44"/>
+      <c r="J102" s="44"/>
+      <c r="K102" s="44"/>
+      <c r="L102" s="44"/>
+      <c r="M102" s="44"/>
+      <c r="N102" s="44"/>
+      <c r="O102" s="44"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B103" s="65"/>
-      <c r="C103" s="65"/>
-      <c r="D103" s="65"/>
-      <c r="E103" s="65"/>
-      <c r="F103" s="65"/>
-      <c r="G103" s="65"/>
-      <c r="H103" s="65"/>
-      <c r="I103" s="65"/>
-      <c r="J103" s="65"/>
-      <c r="K103" s="65"/>
-      <c r="L103" s="65"/>
-      <c r="M103" s="65"/>
-      <c r="N103" s="65"/>
-      <c r="O103" s="65"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="44"/>
+      <c r="G103" s="44"/>
+      <c r="H103" s="44"/>
+      <c r="I103" s="44"/>
+      <c r="J103" s="44"/>
+      <c r="K103" s="44"/>
+      <c r="L103" s="44"/>
+      <c r="M103" s="44"/>
+      <c r="N103" s="44"/>
+      <c r="O103" s="44"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104" s="65"/>
-      <c r="C104" s="65"/>
-      <c r="D104" s="65"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="65"/>
-      <c r="G104" s="65"/>
-      <c r="H104" s="65"/>
-      <c r="I104" s="65"/>
-      <c r="J104" s="65"/>
-      <c r="K104" s="65"/>
-      <c r="L104" s="65"/>
-      <c r="M104" s="65"/>
-      <c r="N104" s="65"/>
-      <c r="O104" s="65"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="44"/>
+      <c r="I104" s="44"/>
+      <c r="J104" s="44"/>
+      <c r="K104" s="44"/>
+      <c r="L104" s="44"/>
+      <c r="M104" s="44"/>
+      <c r="N104" s="44"/>
+      <c r="O104" s="44"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105" s="65"/>
-      <c r="C105" s="65"/>
-      <c r="D105" s="65"/>
-      <c r="E105" s="65"/>
-      <c r="F105" s="65"/>
-      <c r="G105" s="65"/>
-      <c r="H105" s="65"/>
-      <c r="I105" s="65"/>
-      <c r="J105" s="65"/>
-      <c r="K105" s="65"/>
-      <c r="L105" s="65"/>
-      <c r="M105" s="65"/>
-      <c r="N105" s="65"/>
-      <c r="O105" s="65"/>
+      <c r="B105" s="44"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="44"/>
+      <c r="E105" s="44"/>
+      <c r="F105" s="44"/>
+      <c r="G105" s="44"/>
+      <c r="H105" s="44"/>
+      <c r="I105" s="44"/>
+      <c r="J105" s="44"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="44"/>
+      <c r="M105" s="44"/>
+      <c r="N105" s="44"/>
+      <c r="O105" s="44"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="65"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="65"/>
-      <c r="G106" s="65"/>
-      <c r="H106" s="65"/>
-      <c r="I106" s="65"/>
-      <c r="J106" s="65"/>
-      <c r="K106" s="65"/>
-      <c r="L106" s="65"/>
-      <c r="M106" s="65"/>
-      <c r="N106" s="65"/>
-      <c r="O106" s="65"/>
+      <c r="B106" s="44"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="44"/>
+      <c r="H106" s="44"/>
+      <c r="I106" s="44"/>
+      <c r="J106" s="44"/>
+      <c r="K106" s="44"/>
+      <c r="L106" s="44"/>
+      <c r="M106" s="44"/>
+      <c r="N106" s="44"/>
+      <c r="O106" s="44"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="65"/>
-      <c r="C107" s="65"/>
-      <c r="D107" s="65"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="65"/>
-      <c r="G107" s="65"/>
-      <c r="H107" s="65"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="65"/>
-      <c r="K107" s="65"/>
-      <c r="L107" s="65"/>
-      <c r="M107" s="65"/>
-      <c r="N107" s="65"/>
-      <c r="O107" s="65"/>
+      <c r="B107" s="44"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
+      <c r="E107" s="44"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44"/>
+      <c r="H107" s="44"/>
+      <c r="I107" s="44"/>
+      <c r="J107" s="44"/>
+      <c r="K107" s="44"/>
+      <c r="L107" s="44"/>
+      <c r="M107" s="44"/>
+      <c r="N107" s="44"/>
+      <c r="O107" s="44"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="65"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="65"/>
-      <c r="F108" s="65"/>
-      <c r="G108" s="65"/>
-      <c r="H108" s="65"/>
-      <c r="I108" s="65"/>
-      <c r="J108" s="65"/>
-      <c r="K108" s="65"/>
-      <c r="L108" s="65"/>
-      <c r="M108" s="65"/>
-      <c r="N108" s="65"/>
-      <c r="O108" s="65"/>
+      <c r="B108" s="44"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="44"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="44"/>
+      <c r="H108" s="44"/>
+      <c r="I108" s="44"/>
+      <c r="J108" s="44"/>
+      <c r="K108" s="44"/>
+      <c r="L108" s="44"/>
+      <c r="M108" s="44"/>
+      <c r="N108" s="44"/>
+      <c r="O108" s="44"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="65"/>
-      <c r="C109" s="65"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="65"/>
-      <c r="F109" s="65"/>
-      <c r="G109" s="65"/>
-      <c r="H109" s="65"/>
-      <c r="I109" s="65"/>
-      <c r="J109" s="65"/>
-      <c r="K109" s="65"/>
-      <c r="L109" s="65"/>
-      <c r="M109" s="65"/>
-      <c r="N109" s="65"/>
-      <c r="O109" s="65"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
+      <c r="E109" s="44"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="44"/>
+      <c r="H109" s="44"/>
+      <c r="I109" s="44"/>
+      <c r="J109" s="44"/>
+      <c r="K109" s="44"/>
+      <c r="L109" s="44"/>
+      <c r="M109" s="44"/>
+      <c r="N109" s="44"/>
+      <c r="O109" s="44"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B110" s="65"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="65"/>
-      <c r="G110" s="65"/>
-      <c r="H110" s="65"/>
-      <c r="I110" s="65"/>
-      <c r="J110" s="65"/>
-      <c r="K110" s="65"/>
-      <c r="L110" s="65"/>
-      <c r="M110" s="65"/>
-      <c r="N110" s="65"/>
-      <c r="O110" s="65"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="44"/>
+      <c r="I110" s="44"/>
+      <c r="J110" s="44"/>
+      <c r="K110" s="44"/>
+      <c r="L110" s="44"/>
+      <c r="M110" s="44"/>
+      <c r="N110" s="44"/>
+      <c r="O110" s="44"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B111" s="65"/>
-      <c r="C111" s="65"/>
-      <c r="D111" s="65"/>
-      <c r="E111" s="65"/>
-      <c r="F111" s="65"/>
-      <c r="G111" s="65"/>
-      <c r="H111" s="65"/>
-      <c r="I111" s="65"/>
-      <c r="J111" s="65"/>
-      <c r="K111" s="65"/>
-      <c r="L111" s="65"/>
-      <c r="M111" s="65"/>
-      <c r="N111" s="65"/>
-      <c r="O111" s="65"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
+      <c r="H111" s="44"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="44"/>
+      <c r="K111" s="44"/>
+      <c r="L111" s="44"/>
+      <c r="M111" s="44"/>
+      <c r="N111" s="44"/>
+      <c r="O111" s="44"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="65"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="65"/>
-      <c r="E112" s="65"/>
-      <c r="F112" s="65"/>
-      <c r="G112" s="65"/>
-      <c r="H112" s="65"/>
-      <c r="I112" s="65"/>
-      <c r="J112" s="65"/>
-      <c r="K112" s="65"/>
-      <c r="L112" s="65"/>
-      <c r="M112" s="65"/>
-      <c r="N112" s="65"/>
-      <c r="O112" s="65"/>
+      <c r="B112" s="44"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
+      <c r="I112" s="44"/>
+      <c r="J112" s="44"/>
+      <c r="K112" s="44"/>
+      <c r="L112" s="44"/>
+      <c r="M112" s="44"/>
+      <c r="N112" s="44"/>
+      <c r="O112" s="44"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="65"/>
-      <c r="C113" s="65"/>
-      <c r="D113" s="65"/>
-      <c r="E113" s="65"/>
-      <c r="F113" s="65"/>
-      <c r="G113" s="65"/>
-      <c r="H113" s="65"/>
-      <c r="I113" s="65"/>
-      <c r="J113" s="65"/>
-      <c r="K113" s="65"/>
-      <c r="L113" s="65"/>
-      <c r="M113" s="65"/>
-      <c r="N113" s="65"/>
-      <c r="O113" s="65"/>
+      <c r="B113" s="44"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="44"/>
+      <c r="L113" s="44"/>
+      <c r="M113" s="44"/>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="65"/>
-      <c r="C114" s="65"/>
-      <c r="D114" s="65"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="65"/>
-      <c r="G114" s="65"/>
-      <c r="H114" s="65"/>
-      <c r="I114" s="65"/>
-      <c r="J114" s="65"/>
-      <c r="K114" s="65"/>
-      <c r="L114" s="65"/>
-      <c r="M114" s="65"/>
-      <c r="N114" s="65"/>
-      <c r="O114" s="65"/>
+      <c r="B114" s="44"/>
+      <c r="C114" s="44"/>
+      <c r="D114" s="44"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="44"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="44"/>
+      <c r="K114" s="44"/>
+      <c r="L114" s="44"/>
+      <c r="M114" s="44"/>
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
     </row>
     <row r="115" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="65"/>
-      <c r="C115" s="65"/>
-      <c r="D115" s="65"/>
-      <c r="E115" s="65"/>
-      <c r="F115" s="65"/>
-      <c r="G115" s="65"/>
-      <c r="H115" s="65"/>
-      <c r="I115" s="65"/>
-      <c r="J115" s="65"/>
-      <c r="K115" s="65"/>
-      <c r="L115" s="65"/>
-      <c r="M115" s="65"/>
-      <c r="N115" s="65"/>
-      <c r="O115" s="65"/>
+      <c r="B115" s="44"/>
+      <c r="C115" s="44"/>
+      <c r="D115" s="44"/>
+      <c r="E115" s="44"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="44"/>
+      <c r="H115" s="44"/>
+      <c r="I115" s="44"/>
+      <c r="J115" s="44"/>
+      <c r="K115" s="44"/>
+      <c r="L115" s="44"/>
+      <c r="M115" s="44"/>
+      <c r="N115" s="44"/>
+      <c r="O115" s="44"/>
     </row>
     <row r="116" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="40"/>
@@ -4538,38 +4522,38 @@
     </row>
     <row r="117" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="C118" s="66"/>
-      <c r="D118" s="66"/>
-      <c r="E118" s="66"/>
-      <c r="F118" s="66"/>
-      <c r="G118" s="66"/>
-      <c r="H118" s="66"/>
-      <c r="I118" s="66"/>
-      <c r="J118" s="66"/>
-      <c r="K118" s="66"/>
-      <c r="L118" s="66"/>
-      <c r="M118" s="66"/>
-      <c r="N118" s="66"/>
-      <c r="O118" s="66"/>
+      <c r="B118" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C118" s="45"/>
+      <c r="D118" s="45"/>
+      <c r="E118" s="45"/>
+      <c r="F118" s="45"/>
+      <c r="G118" s="45"/>
+      <c r="H118" s="45"/>
+      <c r="I118" s="45"/>
+      <c r="J118" s="45"/>
+      <c r="K118" s="45"/>
+      <c r="L118" s="45"/>
+      <c r="M118" s="45"/>
+      <c r="N118" s="45"/>
+      <c r="O118" s="45"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="66"/>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
-      <c r="L119" s="66"/>
-      <c r="M119" s="66"/>
-      <c r="N119" s="66"/>
-      <c r="O119" s="66"/>
+      <c r="B119" s="45"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="45"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="45"/>
+      <c r="I119" s="45"/>
+      <c r="J119" s="45"/>
+      <c r="K119" s="45"/>
+      <c r="L119" s="45"/>
+      <c r="M119" s="45"/>
+      <c r="N119" s="45"/>
+      <c r="O119" s="45"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25"/>
@@ -4577,24 +4561,6 @@
     <row r="123" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B72:H115"/>
-    <mergeCell ref="I72:O115"/>
-    <mergeCell ref="B118:O119"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="B70:O70"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="I38:O38"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="B42:O42"/>
-    <mergeCell ref="F45:G45"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="A6:O6"/>
     <mergeCell ref="B17:O17"/>
@@ -4611,6 +4577,24 @@
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="H14:L14"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="B42:O42"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B72:H115"/>
+    <mergeCell ref="I72:O115"/>
+    <mergeCell ref="B118:O119"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="B70:O70"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="I38:O38"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Improve navigation UI and fix reference form logic
Enhanced the navigation bar with improved styling, transitions, and hover effects for a more modern UI. Fixed logic in the update references form by correcting the use of Blade curly braces in :disabled and :class attributes. Updated and added several Excel and Word files in the reports and forms directories.
</commit_message>
<xml_diff>
--- a/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
+++ b/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\personal-info-management-system\resources\views\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD105D5-8763-47F7-9620-F53C86EA3E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7350AE26-EBF7-4A43-BE62-9B0EFCF407ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
+    <workbookView xWindow="-28920" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>Civil Service Form No. 6</t>
   </si>
@@ -926,9 +926,6 @@
   </si>
   <si>
     <t>DEPED/Plaridel CS/Baybay 6</t>
-  </si>
-  <si>
-    <t>Feverish and Headache</t>
   </si>
   <si>
     <t>Region VIII (Eastern Visayas)</t>
@@ -1390,6 +1387,87 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1399,15 +1477,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1430,78 +1499,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1874,8 +1871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27B6FB-8E85-4B80-9281-508316E41DF7}">
   <dimension ref="A1:WVX123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25:O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2923,121 +2920,121 @@
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="72"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="72"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="50"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
     </row>
     <row r="9" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+      <c r="N10" s="75"/>
+      <c r="O10" s="75"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -3049,38 +3046,38 @@
       <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52" t="s">
+      <c r="H11" s="76"/>
+      <c r="I11" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52" t="s">
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="53"/>
+      <c r="O11" s="77"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="56"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="80"/>
     </row>
     <row r="13" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
@@ -3109,11 +3106,11 @@
       <c r="G14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
       <c r="M14" s="14"/>
       <c r="N14" s="6" t="s">
         <v>13</v>
@@ -3138,22 +3135,22 @@
     </row>
     <row r="16" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="48"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="68"/>
     </row>
     <row r="18" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
@@ -3268,10 +3265,8 @@
         <v>28</v>
       </c>
       <c r="M25" s="21"/>
-      <c r="N25" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="O25" s="44"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="71"/>
     </row>
     <row r="26" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
@@ -3380,8 +3375,8 @@
       <c r="E33" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
       <c r="H33" s="22"/>
       <c r="I33" s="8"/>
       <c r="J33" s="20"/>
@@ -3429,9 +3424,9 @@
     </row>
     <row r="36" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="22"/>
       <c r="I36" s="8"/>
       <c r="J36" s="20"/>
@@ -3457,32 +3452,32 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
-      <c r="E38" s="58">
+      <c r="E38" s="61">
         <v>45330</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="62"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="79"/>
-      <c r="K38" s="79"/>
-      <c r="L38" s="79"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="79"/>
-      <c r="O38" s="80"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="58"/>
+      <c r="L38" s="58"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="59"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="60" t="s">
+      <c r="I39" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="61"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="62"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="65"/>
     </row>
     <row r="40" spans="2:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
@@ -3502,22 +3497,22 @@
     </row>
     <row r="41" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="46" t="s">
+      <c r="B42" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="47"/>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
-      <c r="I42" s="47"/>
-      <c r="J42" s="47"/>
-      <c r="K42" s="47"/>
-      <c r="L42" s="47"/>
-      <c r="M42" s="47"/>
-      <c r="N42" s="47"/>
-      <c r="O42" s="48"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="68"/>
     </row>
     <row r="43" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -3545,8 +3540,8 @@
       <c r="E45" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
       <c r="H45" s="21"/>
       <c r="I45" s="8"/>
       <c r="O45" s="22"/>
@@ -3635,31 +3630,31 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="E53" s="76"/>
-      <c r="F53" s="76"/>
-      <c r="G53" s="76"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="55"/>
+      <c r="G53" s="55"/>
       <c r="I53" s="8"/>
-      <c r="L53" s="76"/>
-      <c r="M53" s="76"/>
-      <c r="N53" s="76"/>
-      <c r="O53" s="77"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="56"/>
     </row>
     <row r="54" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
-      <c r="E54" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
+      <c r="E54" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="F54" s="47"/>
+      <c r="G54" s="47"/>
       <c r="I54" s="38"/>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
-      <c r="L54" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="M54" s="68"/>
-      <c r="N54" s="68"/>
-      <c r="O54" s="69"/>
+      <c r="L54" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="M54" s="47"/>
+      <c r="N54" s="47"/>
+      <c r="O54" s="48"/>
     </row>
     <row r="55" spans="2:15" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
@@ -3688,7 +3683,7 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
@@ -3697,9 +3692,9 @@
       <c r="O56" s="27"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="70"/>
-      <c r="C57" s="71"/>
-      <c r="D57" s="71"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
       <c r="E57" s="21" t="s">
         <v>63</v>
       </c>
@@ -3738,22 +3733,22 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
-      <c r="G61" s="71"/>
-      <c r="H61" s="71"/>
-      <c r="I61" s="71"/>
-      <c r="J61" s="71"/>
-      <c r="K61" s="71"/>
-      <c r="L61" s="71"/>
+      <c r="G61" s="50"/>
+      <c r="H61" s="50"/>
+      <c r="I61" s="50"/>
+      <c r="J61" s="50"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="50"/>
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
-      <c r="G62" s="72"/>
-      <c r="H62" s="72"/>
-      <c r="I62" s="72"/>
-      <c r="J62" s="72"/>
-      <c r="K62" s="72"/>
-      <c r="L62" s="72"/>
+      <c r="G62" s="51"/>
+      <c r="H62" s="51"/>
+      <c r="I62" s="51"/>
+      <c r="J62" s="51"/>
+      <c r="K62" s="51"/>
+      <c r="L62" s="51"/>
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3779,731 +3774,731 @@
     <row r="68" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="73" t="s">
+      <c r="B70" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="74"/>
-      <c r="F70" s="74"/>
-      <c r="G70" s="74"/>
-      <c r="H70" s="74"/>
-      <c r="I70" s="74"/>
-      <c r="J70" s="74"/>
-      <c r="K70" s="74"/>
-      <c r="L70" s="74"/>
-      <c r="M70" s="74"/>
-      <c r="N70" s="74"/>
-      <c r="O70" s="75"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
+      <c r="H70" s="53"/>
+      <c r="I70" s="53"/>
+      <c r="J70" s="53"/>
+      <c r="K70" s="53"/>
+      <c r="L70" s="53"/>
+      <c r="M70" s="53"/>
+      <c r="N70" s="53"/>
+      <c r="O70" s="54"/>
     </row>
     <row r="71" spans="2:15" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="64" t="s">
+      <c r="B72" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="65"/>
-      <c r="D72" s="65"/>
-      <c r="E72" s="65"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="65"/>
-      <c r="H72" s="65"/>
-      <c r="I72" s="64" t="s">
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
+      <c r="E72" s="44"/>
+      <c r="F72" s="44"/>
+      <c r="G72" s="44"/>
+      <c r="H72" s="44"/>
+      <c r="I72" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="J72" s="65"/>
-      <c r="K72" s="65"/>
-      <c r="L72" s="65"/>
-      <c r="M72" s="65"/>
-      <c r="N72" s="65"/>
-      <c r="O72" s="65"/>
+      <c r="J72" s="44"/>
+      <c r="K72" s="44"/>
+      <c r="L72" s="44"/>
+      <c r="M72" s="44"/>
+      <c r="N72" s="44"/>
+      <c r="O72" s="44"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="65"/>
-      <c r="C73" s="65"/>
-      <c r="D73" s="65"/>
-      <c r="E73" s="65"/>
-      <c r="F73" s="65"/>
-      <c r="G73" s="65"/>
-      <c r="H73" s="65"/>
-      <c r="I73" s="65"/>
-      <c r="J73" s="65"/>
-      <c r="K73" s="65"/>
-      <c r="L73" s="65"/>
-      <c r="M73" s="65"/>
-      <c r="N73" s="65"/>
-      <c r="O73" s="65"/>
+      <c r="B73" s="44"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="44"/>
+      <c r="K73" s="44"/>
+      <c r="L73" s="44"/>
+      <c r="M73" s="44"/>
+      <c r="N73" s="44"/>
+      <c r="O73" s="44"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="65"/>
-      <c r="C74" s="65"/>
-      <c r="D74" s="65"/>
-      <c r="E74" s="65"/>
-      <c r="F74" s="65"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="65"/>
-      <c r="I74" s="65"/>
-      <c r="J74" s="65"/>
-      <c r="K74" s="65"/>
-      <c r="L74" s="65"/>
-      <c r="M74" s="65"/>
-      <c r="N74" s="65"/>
-      <c r="O74" s="65"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="44"/>
+      <c r="G74" s="44"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
+      <c r="J74" s="44"/>
+      <c r="K74" s="44"/>
+      <c r="L74" s="44"/>
+      <c r="M74" s="44"/>
+      <c r="N74" s="44"/>
+      <c r="O74" s="44"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="65"/>
-      <c r="C75" s="65"/>
-      <c r="D75" s="65"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="65"/>
-      <c r="G75" s="65"/>
-      <c r="H75" s="65"/>
-      <c r="I75" s="65"/>
-      <c r="J75" s="65"/>
-      <c r="K75" s="65"/>
-      <c r="L75" s="65"/>
-      <c r="M75" s="65"/>
-      <c r="N75" s="65"/>
-      <c r="O75" s="65"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="44"/>
+      <c r="F75" s="44"/>
+      <c r="G75" s="44"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="44"/>
+      <c r="J75" s="44"/>
+      <c r="K75" s="44"/>
+      <c r="L75" s="44"/>
+      <c r="M75" s="44"/>
+      <c r="N75" s="44"/>
+      <c r="O75" s="44"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="65"/>
-      <c r="C76" s="65"/>
-      <c r="D76" s="65"/>
-      <c r="E76" s="65"/>
-      <c r="F76" s="65"/>
-      <c r="G76" s="65"/>
-      <c r="H76" s="65"/>
-      <c r="I76" s="65"/>
-      <c r="J76" s="65"/>
-      <c r="K76" s="65"/>
-      <c r="L76" s="65"/>
-      <c r="M76" s="65"/>
-      <c r="N76" s="65"/>
-      <c r="O76" s="65"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="44"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
+      <c r="J76" s="44"/>
+      <c r="K76" s="44"/>
+      <c r="L76" s="44"/>
+      <c r="M76" s="44"/>
+      <c r="N76" s="44"/>
+      <c r="O76" s="44"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="65"/>
-      <c r="C77" s="65"/>
-      <c r="D77" s="65"/>
-      <c r="E77" s="65"/>
-      <c r="F77" s="65"/>
-      <c r="G77" s="65"/>
-      <c r="H77" s="65"/>
-      <c r="I77" s="65"/>
-      <c r="J77" s="65"/>
-      <c r="K77" s="65"/>
-      <c r="L77" s="65"/>
-      <c r="M77" s="65"/>
-      <c r="N77" s="65"/>
-      <c r="O77" s="65"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
+      <c r="J77" s="44"/>
+      <c r="K77" s="44"/>
+      <c r="L77" s="44"/>
+      <c r="M77" s="44"/>
+      <c r="N77" s="44"/>
+      <c r="O77" s="44"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="65"/>
-      <c r="C78" s="65"/>
-      <c r="D78" s="65"/>
-      <c r="E78" s="65"/>
-      <c r="F78" s="65"/>
-      <c r="G78" s="65"/>
-      <c r="H78" s="65"/>
-      <c r="I78" s="65"/>
-      <c r="J78" s="65"/>
-      <c r="K78" s="65"/>
-      <c r="L78" s="65"/>
-      <c r="M78" s="65"/>
-      <c r="N78" s="65"/>
-      <c r="O78" s="65"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="44"/>
+      <c r="J78" s="44"/>
+      <c r="K78" s="44"/>
+      <c r="L78" s="44"/>
+      <c r="M78" s="44"/>
+      <c r="N78" s="44"/>
+      <c r="O78" s="44"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="65"/>
-      <c r="C79" s="65"/>
-      <c r="D79" s="65"/>
-      <c r="E79" s="65"/>
-      <c r="F79" s="65"/>
-      <c r="G79" s="65"/>
-      <c r="H79" s="65"/>
-      <c r="I79" s="65"/>
-      <c r="J79" s="65"/>
-      <c r="K79" s="65"/>
-      <c r="L79" s="65"/>
-      <c r="M79" s="65"/>
-      <c r="N79" s="65"/>
-      <c r="O79" s="65"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
+      <c r="I79" s="44"/>
+      <c r="J79" s="44"/>
+      <c r="K79" s="44"/>
+      <c r="L79" s="44"/>
+      <c r="M79" s="44"/>
+      <c r="N79" s="44"/>
+      <c r="O79" s="44"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="65"/>
-      <c r="C80" s="65"/>
-      <c r="D80" s="65"/>
-      <c r="E80" s="65"/>
-      <c r="F80" s="65"/>
-      <c r="G80" s="65"/>
-      <c r="H80" s="65"/>
-      <c r="I80" s="65"/>
-      <c r="J80" s="65"/>
-      <c r="K80" s="65"/>
-      <c r="L80" s="65"/>
-      <c r="M80" s="65"/>
-      <c r="N80" s="65"/>
-      <c r="O80" s="65"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="44"/>
+      <c r="L80" s="44"/>
+      <c r="M80" s="44"/>
+      <c r="N80" s="44"/>
+      <c r="O80" s="44"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="65"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="65"/>
-      <c r="E81" s="65"/>
-      <c r="F81" s="65"/>
-      <c r="G81" s="65"/>
-      <c r="H81" s="65"/>
-      <c r="I81" s="65"/>
-      <c r="J81" s="65"/>
-      <c r="K81" s="65"/>
-      <c r="L81" s="65"/>
-      <c r="M81" s="65"/>
-      <c r="N81" s="65"/>
-      <c r="O81" s="65"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="44"/>
+      <c r="J81" s="44"/>
+      <c r="K81" s="44"/>
+      <c r="L81" s="44"/>
+      <c r="M81" s="44"/>
+      <c r="N81" s="44"/>
+      <c r="O81" s="44"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="65"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="65"/>
-      <c r="E82" s="65"/>
-      <c r="F82" s="65"/>
-      <c r="G82" s="65"/>
-      <c r="H82" s="65"/>
-      <c r="I82" s="65"/>
-      <c r="J82" s="65"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
-      <c r="M82" s="65"/>
-      <c r="N82" s="65"/>
-      <c r="O82" s="65"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="44"/>
+      <c r="K82" s="44"/>
+      <c r="L82" s="44"/>
+      <c r="M82" s="44"/>
+      <c r="N82" s="44"/>
+      <c r="O82" s="44"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="65"/>
-      <c r="C83" s="65"/>
-      <c r="D83" s="65"/>
-      <c r="E83" s="65"/>
-      <c r="F83" s="65"/>
-      <c r="G83" s="65"/>
-      <c r="H83" s="65"/>
-      <c r="I83" s="65"/>
-      <c r="J83" s="65"/>
-      <c r="K83" s="65"/>
-      <c r="L83" s="65"/>
-      <c r="M83" s="65"/>
-      <c r="N83" s="65"/>
-      <c r="O83" s="65"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="44"/>
+      <c r="L83" s="44"/>
+      <c r="M83" s="44"/>
+      <c r="N83" s="44"/>
+      <c r="O83" s="44"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="65"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="65"/>
-      <c r="E84" s="65"/>
-      <c r="F84" s="65"/>
-      <c r="G84" s="65"/>
-      <c r="H84" s="65"/>
-      <c r="I84" s="65"/>
-      <c r="J84" s="65"/>
-      <c r="K84" s="65"/>
-      <c r="L84" s="65"/>
-      <c r="M84" s="65"/>
-      <c r="N84" s="65"/>
-      <c r="O84" s="65"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
+      <c r="J84" s="44"/>
+      <c r="K84" s="44"/>
+      <c r="L84" s="44"/>
+      <c r="M84" s="44"/>
+      <c r="N84" s="44"/>
+      <c r="O84" s="44"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="65"/>
-      <c r="C85" s="65"/>
-      <c r="D85" s="65"/>
-      <c r="E85" s="65"/>
-      <c r="F85" s="65"/>
-      <c r="G85" s="65"/>
-      <c r="H85" s="65"/>
-      <c r="I85" s="65"/>
-      <c r="J85" s="65"/>
-      <c r="K85" s="65"/>
-      <c r="L85" s="65"/>
-      <c r="M85" s="65"/>
-      <c r="N85" s="65"/>
-      <c r="O85" s="65"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44"/>
+      <c r="J85" s="44"/>
+      <c r="K85" s="44"/>
+      <c r="L85" s="44"/>
+      <c r="M85" s="44"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="44"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="65"/>
-      <c r="C86" s="65"/>
-      <c r="D86" s="65"/>
-      <c r="E86" s="65"/>
-      <c r="F86" s="65"/>
-      <c r="G86" s="65"/>
-      <c r="H86" s="65"/>
-      <c r="I86" s="65"/>
-      <c r="J86" s="65"/>
-      <c r="K86" s="65"/>
-      <c r="L86" s="65"/>
-      <c r="M86" s="65"/>
-      <c r="N86" s="65"/>
-      <c r="O86" s="65"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44"/>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="44"/>
+      <c r="J86" s="44"/>
+      <c r="K86" s="44"/>
+      <c r="L86" s="44"/>
+      <c r="M86" s="44"/>
+      <c r="N86" s="44"/>
+      <c r="O86" s="44"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="65"/>
-      <c r="C87" s="65"/>
-      <c r="D87" s="65"/>
-      <c r="E87" s="65"/>
-      <c r="F87" s="65"/>
-      <c r="G87" s="65"/>
-      <c r="H87" s="65"/>
-      <c r="I87" s="65"/>
-      <c r="J87" s="65"/>
-      <c r="K87" s="65"/>
-      <c r="L87" s="65"/>
-      <c r="M87" s="65"/>
-      <c r="N87" s="65"/>
-      <c r="O87" s="65"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
+      <c r="J87" s="44"/>
+      <c r="K87" s="44"/>
+      <c r="L87" s="44"/>
+      <c r="M87" s="44"/>
+      <c r="N87" s="44"/>
+      <c r="O87" s="44"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="65"/>
-      <c r="C88" s="65"/>
-      <c r="D88" s="65"/>
-      <c r="E88" s="65"/>
-      <c r="F88" s="65"/>
-      <c r="G88" s="65"/>
-      <c r="H88" s="65"/>
-      <c r="I88" s="65"/>
-      <c r="J88" s="65"/>
-      <c r="K88" s="65"/>
-      <c r="L88" s="65"/>
-      <c r="M88" s="65"/>
-      <c r="N88" s="65"/>
-      <c r="O88" s="65"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="44"/>
+      <c r="J88" s="44"/>
+      <c r="K88" s="44"/>
+      <c r="L88" s="44"/>
+      <c r="M88" s="44"/>
+      <c r="N88" s="44"/>
+      <c r="O88" s="44"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="65"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="65"/>
-      <c r="E89" s="65"/>
-      <c r="F89" s="65"/>
-      <c r="G89" s="65"/>
-      <c r="H89" s="65"/>
-      <c r="I89" s="65"/>
-      <c r="J89" s="65"/>
-      <c r="K89" s="65"/>
-      <c r="L89" s="65"/>
-      <c r="M89" s="65"/>
-      <c r="N89" s="65"/>
-      <c r="O89" s="65"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="44"/>
+      <c r="I89" s="44"/>
+      <c r="J89" s="44"/>
+      <c r="K89" s="44"/>
+      <c r="L89" s="44"/>
+      <c r="M89" s="44"/>
+      <c r="N89" s="44"/>
+      <c r="O89" s="44"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="65"/>
-      <c r="C90" s="65"/>
-      <c r="D90" s="65"/>
-      <c r="E90" s="65"/>
-      <c r="F90" s="65"/>
-      <c r="G90" s="65"/>
-      <c r="H90" s="65"/>
-      <c r="I90" s="65"/>
-      <c r="J90" s="65"/>
-      <c r="K90" s="65"/>
-      <c r="L90" s="65"/>
-      <c r="M90" s="65"/>
-      <c r="N90" s="65"/>
-      <c r="O90" s="65"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44"/>
+      <c r="E90" s="44"/>
+      <c r="F90" s="44"/>
+      <c r="G90" s="44"/>
+      <c r="H90" s="44"/>
+      <c r="I90" s="44"/>
+      <c r="J90" s="44"/>
+      <c r="K90" s="44"/>
+      <c r="L90" s="44"/>
+      <c r="M90" s="44"/>
+      <c r="N90" s="44"/>
+      <c r="O90" s="44"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="65"/>
-      <c r="C91" s="65"/>
-      <c r="D91" s="65"/>
-      <c r="E91" s="65"/>
-      <c r="F91" s="65"/>
-      <c r="G91" s="65"/>
-      <c r="H91" s="65"/>
-      <c r="I91" s="65"/>
-      <c r="J91" s="65"/>
-      <c r="K91" s="65"/>
-      <c r="L91" s="65"/>
-      <c r="M91" s="65"/>
-      <c r="N91" s="65"/>
-      <c r="O91" s="65"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44"/>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="44"/>
+      <c r="I91" s="44"/>
+      <c r="J91" s="44"/>
+      <c r="K91" s="44"/>
+      <c r="L91" s="44"/>
+      <c r="M91" s="44"/>
+      <c r="N91" s="44"/>
+      <c r="O91" s="44"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="65"/>
-      <c r="C92" s="65"/>
-      <c r="D92" s="65"/>
-      <c r="E92" s="65"/>
-      <c r="F92" s="65"/>
-      <c r="G92" s="65"/>
-      <c r="H92" s="65"/>
-      <c r="I92" s="65"/>
-      <c r="J92" s="65"/>
-      <c r="K92" s="65"/>
-      <c r="L92" s="65"/>
-      <c r="M92" s="65"/>
-      <c r="N92" s="65"/>
-      <c r="O92" s="65"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44"/>
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="44"/>
+      <c r="I92" s="44"/>
+      <c r="J92" s="44"/>
+      <c r="K92" s="44"/>
+      <c r="L92" s="44"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="44"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="65"/>
-      <c r="C93" s="65"/>
-      <c r="D93" s="65"/>
-      <c r="E93" s="65"/>
-      <c r="F93" s="65"/>
-      <c r="G93" s="65"/>
-      <c r="H93" s="65"/>
-      <c r="I93" s="65"/>
-      <c r="J93" s="65"/>
-      <c r="K93" s="65"/>
-      <c r="L93" s="65"/>
-      <c r="M93" s="65"/>
-      <c r="N93" s="65"/>
-      <c r="O93" s="65"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="44"/>
+      <c r="I93" s="44"/>
+      <c r="J93" s="44"/>
+      <c r="K93" s="44"/>
+      <c r="L93" s="44"/>
+      <c r="M93" s="44"/>
+      <c r="N93" s="44"/>
+      <c r="O93" s="44"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="65"/>
-      <c r="C94" s="65"/>
-      <c r="D94" s="65"/>
-      <c r="E94" s="65"/>
-      <c r="F94" s="65"/>
-      <c r="G94" s="65"/>
-      <c r="H94" s="65"/>
-      <c r="I94" s="65"/>
-      <c r="J94" s="65"/>
-      <c r="K94" s="65"/>
-      <c r="L94" s="65"/>
-      <c r="M94" s="65"/>
-      <c r="N94" s="65"/>
-      <c r="O94" s="65"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
+      <c r="D94" s="44"/>
+      <c r="E94" s="44"/>
+      <c r="F94" s="44"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="44"/>
+      <c r="I94" s="44"/>
+      <c r="J94" s="44"/>
+      <c r="K94" s="44"/>
+      <c r="L94" s="44"/>
+      <c r="M94" s="44"/>
+      <c r="N94" s="44"/>
+      <c r="O94" s="44"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="65"/>
-      <c r="C95" s="65"/>
-      <c r="D95" s="65"/>
-      <c r="E95" s="65"/>
-      <c r="F95" s="65"/>
-      <c r="G95" s="65"/>
-      <c r="H95" s="65"/>
-      <c r="I95" s="65"/>
-      <c r="J95" s="65"/>
-      <c r="K95" s="65"/>
-      <c r="L95" s="65"/>
-      <c r="M95" s="65"/>
-      <c r="N95" s="65"/>
-      <c r="O95" s="65"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="44"/>
+      <c r="H95" s="44"/>
+      <c r="I95" s="44"/>
+      <c r="J95" s="44"/>
+      <c r="K95" s="44"/>
+      <c r="L95" s="44"/>
+      <c r="M95" s="44"/>
+      <c r="N95" s="44"/>
+      <c r="O95" s="44"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B96" s="65"/>
-      <c r="C96" s="65"/>
-      <c r="D96" s="65"/>
-      <c r="E96" s="65"/>
-      <c r="F96" s="65"/>
-      <c r="G96" s="65"/>
-      <c r="H96" s="65"/>
-      <c r="I96" s="65"/>
-      <c r="J96" s="65"/>
-      <c r="K96" s="65"/>
-      <c r="L96" s="65"/>
-      <c r="M96" s="65"/>
-      <c r="N96" s="65"/>
-      <c r="O96" s="65"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44"/>
+      <c r="E96" s="44"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+      <c r="I96" s="44"/>
+      <c r="J96" s="44"/>
+      <c r="K96" s="44"/>
+      <c r="L96" s="44"/>
+      <c r="M96" s="44"/>
+      <c r="N96" s="44"/>
+      <c r="O96" s="44"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97" s="65"/>
-      <c r="C97" s="65"/>
-      <c r="D97" s="65"/>
-      <c r="E97" s="65"/>
-      <c r="F97" s="65"/>
-      <c r="G97" s="65"/>
-      <c r="H97" s="65"/>
-      <c r="I97" s="65"/>
-      <c r="J97" s="65"/>
-      <c r="K97" s="65"/>
-      <c r="L97" s="65"/>
-      <c r="M97" s="65"/>
-      <c r="N97" s="65"/>
-      <c r="O97" s="65"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
+      <c r="E97" s="44"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44"/>
+      <c r="J97" s="44"/>
+      <c r="K97" s="44"/>
+      <c r="L97" s="44"/>
+      <c r="M97" s="44"/>
+      <c r="N97" s="44"/>
+      <c r="O97" s="44"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="65"/>
-      <c r="C98" s="65"/>
-      <c r="D98" s="65"/>
-      <c r="E98" s="65"/>
-      <c r="F98" s="65"/>
-      <c r="G98" s="65"/>
-      <c r="H98" s="65"/>
-      <c r="I98" s="65"/>
-      <c r="J98" s="65"/>
-      <c r="K98" s="65"/>
-      <c r="L98" s="65"/>
-      <c r="M98" s="65"/>
-      <c r="N98" s="65"/>
-      <c r="O98" s="65"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+      <c r="J98" s="44"/>
+      <c r="K98" s="44"/>
+      <c r="L98" s="44"/>
+      <c r="M98" s="44"/>
+      <c r="N98" s="44"/>
+      <c r="O98" s="44"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99" s="65"/>
-      <c r="C99" s="65"/>
-      <c r="D99" s="65"/>
-      <c r="E99" s="65"/>
-      <c r="F99" s="65"/>
-      <c r="G99" s="65"/>
-      <c r="H99" s="65"/>
-      <c r="I99" s="65"/>
-      <c r="J99" s="65"/>
-      <c r="K99" s="65"/>
-      <c r="L99" s="65"/>
-      <c r="M99" s="65"/>
-      <c r="N99" s="65"/>
-      <c r="O99" s="65"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
+      <c r="E99" s="44"/>
+      <c r="F99" s="44"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+      <c r="I99" s="44"/>
+      <c r="J99" s="44"/>
+      <c r="K99" s="44"/>
+      <c r="L99" s="44"/>
+      <c r="M99" s="44"/>
+      <c r="N99" s="44"/>
+      <c r="O99" s="44"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="65"/>
-      <c r="C100" s="65"/>
-      <c r="D100" s="65"/>
-      <c r="E100" s="65"/>
-      <c r="F100" s="65"/>
-      <c r="G100" s="65"/>
-      <c r="H100" s="65"/>
-      <c r="I100" s="65"/>
-      <c r="J100" s="65"/>
-      <c r="K100" s="65"/>
-      <c r="L100" s="65"/>
-      <c r="M100" s="65"/>
-      <c r="N100" s="65"/>
-      <c r="O100" s="65"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+      <c r="E100" s="44"/>
+      <c r="F100" s="44"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+      <c r="I100" s="44"/>
+      <c r="J100" s="44"/>
+      <c r="K100" s="44"/>
+      <c r="L100" s="44"/>
+      <c r="M100" s="44"/>
+      <c r="N100" s="44"/>
+      <c r="O100" s="44"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="65"/>
-      <c r="C101" s="65"/>
-      <c r="D101" s="65"/>
-      <c r="E101" s="65"/>
-      <c r="F101" s="65"/>
-      <c r="G101" s="65"/>
-      <c r="H101" s="65"/>
-      <c r="I101" s="65"/>
-      <c r="J101" s="65"/>
-      <c r="K101" s="65"/>
-      <c r="L101" s="65"/>
-      <c r="M101" s="65"/>
-      <c r="N101" s="65"/>
-      <c r="O101" s="65"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="44"/>
+      <c r="E101" s="44"/>
+      <c r="F101" s="44"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="44"/>
+      <c r="I101" s="44"/>
+      <c r="J101" s="44"/>
+      <c r="K101" s="44"/>
+      <c r="L101" s="44"/>
+      <c r="M101" s="44"/>
+      <c r="N101" s="44"/>
+      <c r="O101" s="44"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B102" s="65"/>
-      <c r="C102" s="65"/>
-      <c r="D102" s="65"/>
-      <c r="E102" s="65"/>
-      <c r="F102" s="65"/>
-      <c r="G102" s="65"/>
-      <c r="H102" s="65"/>
-      <c r="I102" s="65"/>
-      <c r="J102" s="65"/>
-      <c r="K102" s="65"/>
-      <c r="L102" s="65"/>
-      <c r="M102" s="65"/>
-      <c r="N102" s="65"/>
-      <c r="O102" s="65"/>
+      <c r="B102" s="44"/>
+      <c r="C102" s="44"/>
+      <c r="D102" s="44"/>
+      <c r="E102" s="44"/>
+      <c r="F102" s="44"/>
+      <c r="G102" s="44"/>
+      <c r="H102" s="44"/>
+      <c r="I102" s="44"/>
+      <c r="J102" s="44"/>
+      <c r="K102" s="44"/>
+      <c r="L102" s="44"/>
+      <c r="M102" s="44"/>
+      <c r="N102" s="44"/>
+      <c r="O102" s="44"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B103" s="65"/>
-      <c r="C103" s="65"/>
-      <c r="D103" s="65"/>
-      <c r="E103" s="65"/>
-      <c r="F103" s="65"/>
-      <c r="G103" s="65"/>
-      <c r="H103" s="65"/>
-      <c r="I103" s="65"/>
-      <c r="J103" s="65"/>
-      <c r="K103" s="65"/>
-      <c r="L103" s="65"/>
-      <c r="M103" s="65"/>
-      <c r="N103" s="65"/>
-      <c r="O103" s="65"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
+      <c r="E103" s="44"/>
+      <c r="F103" s="44"/>
+      <c r="G103" s="44"/>
+      <c r="H103" s="44"/>
+      <c r="I103" s="44"/>
+      <c r="J103" s="44"/>
+      <c r="K103" s="44"/>
+      <c r="L103" s="44"/>
+      <c r="M103" s="44"/>
+      <c r="N103" s="44"/>
+      <c r="O103" s="44"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104" s="65"/>
-      <c r="C104" s="65"/>
-      <c r="D104" s="65"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="65"/>
-      <c r="G104" s="65"/>
-      <c r="H104" s="65"/>
-      <c r="I104" s="65"/>
-      <c r="J104" s="65"/>
-      <c r="K104" s="65"/>
-      <c r="L104" s="65"/>
-      <c r="M104" s="65"/>
-      <c r="N104" s="65"/>
-      <c r="O104" s="65"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44"/>
+      <c r="E104" s="44"/>
+      <c r="F104" s="44"/>
+      <c r="G104" s="44"/>
+      <c r="H104" s="44"/>
+      <c r="I104" s="44"/>
+      <c r="J104" s="44"/>
+      <c r="K104" s="44"/>
+      <c r="L104" s="44"/>
+      <c r="M104" s="44"/>
+      <c r="N104" s="44"/>
+      <c r="O104" s="44"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105" s="65"/>
-      <c r="C105" s="65"/>
-      <c r="D105" s="65"/>
-      <c r="E105" s="65"/>
-      <c r="F105" s="65"/>
-      <c r="G105" s="65"/>
-      <c r="H105" s="65"/>
-      <c r="I105" s="65"/>
-      <c r="J105" s="65"/>
-      <c r="K105" s="65"/>
-      <c r="L105" s="65"/>
-      <c r="M105" s="65"/>
-      <c r="N105" s="65"/>
-      <c r="O105" s="65"/>
+      <c r="B105" s="44"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="44"/>
+      <c r="E105" s="44"/>
+      <c r="F105" s="44"/>
+      <c r="G105" s="44"/>
+      <c r="H105" s="44"/>
+      <c r="I105" s="44"/>
+      <c r="J105" s="44"/>
+      <c r="K105" s="44"/>
+      <c r="L105" s="44"/>
+      <c r="M105" s="44"/>
+      <c r="N105" s="44"/>
+      <c r="O105" s="44"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="65"/>
-      <c r="C106" s="65"/>
-      <c r="D106" s="65"/>
-      <c r="E106" s="65"/>
-      <c r="F106" s="65"/>
-      <c r="G106" s="65"/>
-      <c r="H106" s="65"/>
-      <c r="I106" s="65"/>
-      <c r="J106" s="65"/>
-      <c r="K106" s="65"/>
-      <c r="L106" s="65"/>
-      <c r="M106" s="65"/>
-      <c r="N106" s="65"/>
-      <c r="O106" s="65"/>
+      <c r="B106" s="44"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="44"/>
+      <c r="E106" s="44"/>
+      <c r="F106" s="44"/>
+      <c r="G106" s="44"/>
+      <c r="H106" s="44"/>
+      <c r="I106" s="44"/>
+      <c r="J106" s="44"/>
+      <c r="K106" s="44"/>
+      <c r="L106" s="44"/>
+      <c r="M106" s="44"/>
+      <c r="N106" s="44"/>
+      <c r="O106" s="44"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="65"/>
-      <c r="C107" s="65"/>
-      <c r="D107" s="65"/>
-      <c r="E107" s="65"/>
-      <c r="F107" s="65"/>
-      <c r="G107" s="65"/>
-      <c r="H107" s="65"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="65"/>
-      <c r="K107" s="65"/>
-      <c r="L107" s="65"/>
-      <c r="M107" s="65"/>
-      <c r="N107" s="65"/>
-      <c r="O107" s="65"/>
+      <c r="B107" s="44"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
+      <c r="E107" s="44"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44"/>
+      <c r="H107" s="44"/>
+      <c r="I107" s="44"/>
+      <c r="J107" s="44"/>
+      <c r="K107" s="44"/>
+      <c r="L107" s="44"/>
+      <c r="M107" s="44"/>
+      <c r="N107" s="44"/>
+      <c r="O107" s="44"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="65"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="65"/>
-      <c r="F108" s="65"/>
-      <c r="G108" s="65"/>
-      <c r="H108" s="65"/>
-      <c r="I108" s="65"/>
-      <c r="J108" s="65"/>
-      <c r="K108" s="65"/>
-      <c r="L108" s="65"/>
-      <c r="M108" s="65"/>
-      <c r="N108" s="65"/>
-      <c r="O108" s="65"/>
+      <c r="B108" s="44"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44"/>
+      <c r="E108" s="44"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="44"/>
+      <c r="H108" s="44"/>
+      <c r="I108" s="44"/>
+      <c r="J108" s="44"/>
+      <c r="K108" s="44"/>
+      <c r="L108" s="44"/>
+      <c r="M108" s="44"/>
+      <c r="N108" s="44"/>
+      <c r="O108" s="44"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="65"/>
-      <c r="C109" s="65"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="65"/>
-      <c r="F109" s="65"/>
-      <c r="G109" s="65"/>
-      <c r="H109" s="65"/>
-      <c r="I109" s="65"/>
-      <c r="J109" s="65"/>
-      <c r="K109" s="65"/>
-      <c r="L109" s="65"/>
-      <c r="M109" s="65"/>
-      <c r="N109" s="65"/>
-      <c r="O109" s="65"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
+      <c r="E109" s="44"/>
+      <c r="F109" s="44"/>
+      <c r="G109" s="44"/>
+      <c r="H109" s="44"/>
+      <c r="I109" s="44"/>
+      <c r="J109" s="44"/>
+      <c r="K109" s="44"/>
+      <c r="L109" s="44"/>
+      <c r="M109" s="44"/>
+      <c r="N109" s="44"/>
+      <c r="O109" s="44"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B110" s="65"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="65"/>
-      <c r="G110" s="65"/>
-      <c r="H110" s="65"/>
-      <c r="I110" s="65"/>
-      <c r="J110" s="65"/>
-      <c r="K110" s="65"/>
-      <c r="L110" s="65"/>
-      <c r="M110" s="65"/>
-      <c r="N110" s="65"/>
-      <c r="O110" s="65"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44"/>
+      <c r="H110" s="44"/>
+      <c r="I110" s="44"/>
+      <c r="J110" s="44"/>
+      <c r="K110" s="44"/>
+      <c r="L110" s="44"/>
+      <c r="M110" s="44"/>
+      <c r="N110" s="44"/>
+      <c r="O110" s="44"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B111" s="65"/>
-      <c r="C111" s="65"/>
-      <c r="D111" s="65"/>
-      <c r="E111" s="65"/>
-      <c r="F111" s="65"/>
-      <c r="G111" s="65"/>
-      <c r="H111" s="65"/>
-      <c r="I111" s="65"/>
-      <c r="J111" s="65"/>
-      <c r="K111" s="65"/>
-      <c r="L111" s="65"/>
-      <c r="M111" s="65"/>
-      <c r="N111" s="65"/>
-      <c r="O111" s="65"/>
+      <c r="B111" s="44"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="44"/>
+      <c r="E111" s="44"/>
+      <c r="F111" s="44"/>
+      <c r="G111" s="44"/>
+      <c r="H111" s="44"/>
+      <c r="I111" s="44"/>
+      <c r="J111" s="44"/>
+      <c r="K111" s="44"/>
+      <c r="L111" s="44"/>
+      <c r="M111" s="44"/>
+      <c r="N111" s="44"/>
+      <c r="O111" s="44"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="65"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="65"/>
-      <c r="E112" s="65"/>
-      <c r="F112" s="65"/>
-      <c r="G112" s="65"/>
-      <c r="H112" s="65"/>
-      <c r="I112" s="65"/>
-      <c r="J112" s="65"/>
-      <c r="K112" s="65"/>
-      <c r="L112" s="65"/>
-      <c r="M112" s="65"/>
-      <c r="N112" s="65"/>
-      <c r="O112" s="65"/>
+      <c r="B112" s="44"/>
+      <c r="C112" s="44"/>
+      <c r="D112" s="44"/>
+      <c r="E112" s="44"/>
+      <c r="F112" s="44"/>
+      <c r="G112" s="44"/>
+      <c r="H112" s="44"/>
+      <c r="I112" s="44"/>
+      <c r="J112" s="44"/>
+      <c r="K112" s="44"/>
+      <c r="L112" s="44"/>
+      <c r="M112" s="44"/>
+      <c r="N112" s="44"/>
+      <c r="O112" s="44"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="65"/>
-      <c r="C113" s="65"/>
-      <c r="D113" s="65"/>
-      <c r="E113" s="65"/>
-      <c r="F113" s="65"/>
-      <c r="G113" s="65"/>
-      <c r="H113" s="65"/>
-      <c r="I113" s="65"/>
-      <c r="J113" s="65"/>
-      <c r="K113" s="65"/>
-      <c r="L113" s="65"/>
-      <c r="M113" s="65"/>
-      <c r="N113" s="65"/>
-      <c r="O113" s="65"/>
+      <c r="B113" s="44"/>
+      <c r="C113" s="44"/>
+      <c r="D113" s="44"/>
+      <c r="E113" s="44"/>
+      <c r="F113" s="44"/>
+      <c r="G113" s="44"/>
+      <c r="H113" s="44"/>
+      <c r="I113" s="44"/>
+      <c r="J113" s="44"/>
+      <c r="K113" s="44"/>
+      <c r="L113" s="44"/>
+      <c r="M113" s="44"/>
+      <c r="N113" s="44"/>
+      <c r="O113" s="44"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="65"/>
-      <c r="C114" s="65"/>
-      <c r="D114" s="65"/>
-      <c r="E114" s="65"/>
-      <c r="F114" s="65"/>
-      <c r="G114" s="65"/>
-      <c r="H114" s="65"/>
-      <c r="I114" s="65"/>
-      <c r="J114" s="65"/>
-      <c r="K114" s="65"/>
-      <c r="L114" s="65"/>
-      <c r="M114" s="65"/>
-      <c r="N114" s="65"/>
-      <c r="O114" s="65"/>
+      <c r="B114" s="44"/>
+      <c r="C114" s="44"/>
+      <c r="D114" s="44"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44"/>
+      <c r="H114" s="44"/>
+      <c r="I114" s="44"/>
+      <c r="J114" s="44"/>
+      <c r="K114" s="44"/>
+      <c r="L114" s="44"/>
+      <c r="M114" s="44"/>
+      <c r="N114" s="44"/>
+      <c r="O114" s="44"/>
     </row>
     <row r="115" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="65"/>
-      <c r="C115" s="65"/>
-      <c r="D115" s="65"/>
-      <c r="E115" s="65"/>
-      <c r="F115" s="65"/>
-      <c r="G115" s="65"/>
-      <c r="H115" s="65"/>
-      <c r="I115" s="65"/>
-      <c r="J115" s="65"/>
-      <c r="K115" s="65"/>
-      <c r="L115" s="65"/>
-      <c r="M115" s="65"/>
-      <c r="N115" s="65"/>
-      <c r="O115" s="65"/>
+      <c r="B115" s="44"/>
+      <c r="C115" s="44"/>
+      <c r="D115" s="44"/>
+      <c r="E115" s="44"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="44"/>
+      <c r="H115" s="44"/>
+      <c r="I115" s="44"/>
+      <c r="J115" s="44"/>
+      <c r="K115" s="44"/>
+      <c r="L115" s="44"/>
+      <c r="M115" s="44"/>
+      <c r="N115" s="44"/>
+      <c r="O115" s="44"/>
     </row>
     <row r="116" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="40"/>
@@ -4523,38 +4518,38 @@
     </row>
     <row r="117" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="66" t="s">
+      <c r="B118" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C118" s="66"/>
-      <c r="D118" s="66"/>
-      <c r="E118" s="66"/>
-      <c r="F118" s="66"/>
-      <c r="G118" s="66"/>
-      <c r="H118" s="66"/>
-      <c r="I118" s="66"/>
-      <c r="J118" s="66"/>
-      <c r="K118" s="66"/>
-      <c r="L118" s="66"/>
-      <c r="M118" s="66"/>
-      <c r="N118" s="66"/>
-      <c r="O118" s="66"/>
+      <c r="C118" s="45"/>
+      <c r="D118" s="45"/>
+      <c r="E118" s="45"/>
+      <c r="F118" s="45"/>
+      <c r="G118" s="45"/>
+      <c r="H118" s="45"/>
+      <c r="I118" s="45"/>
+      <c r="J118" s="45"/>
+      <c r="K118" s="45"/>
+      <c r="L118" s="45"/>
+      <c r="M118" s="45"/>
+      <c r="N118" s="45"/>
+      <c r="O118" s="45"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="66"/>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="66"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
-      <c r="L119" s="66"/>
-      <c r="M119" s="66"/>
-      <c r="N119" s="66"/>
-      <c r="O119" s="66"/>
+      <c r="B119" s="45"/>
+      <c r="C119" s="45"/>
+      <c r="D119" s="45"/>
+      <c r="E119" s="45"/>
+      <c r="F119" s="45"/>
+      <c r="G119" s="45"/>
+      <c r="H119" s="45"/>
+      <c r="I119" s="45"/>
+      <c r="J119" s="45"/>
+      <c r="K119" s="45"/>
+      <c r="L119" s="45"/>
+      <c r="M119" s="45"/>
+      <c r="N119" s="45"/>
+      <c r="O119" s="45"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25"/>
@@ -4562,24 +4557,6 @@
     <row r="123" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B72:H115"/>
-    <mergeCell ref="I72:O115"/>
-    <mergeCell ref="B118:O119"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="B70:O70"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="I38:O38"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="B42:O42"/>
-    <mergeCell ref="F45:G45"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="A6:O6"/>
     <mergeCell ref="B17:O17"/>
@@ -4596,6 +4573,24 @@
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="H14:L14"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="B42:O42"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="B72:H115"/>
+    <mergeCell ref="I72:O115"/>
+    <mergeCell ref="B118:O119"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="B70:O70"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="I38:O38"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Calculate and display day debt at leave request submission for SICK LEAVE and SERVICE CREDIT
Modified LeaveRequestController to calculate day_debt when SICK LEAVE or SERVICE CREDIT requests are submitted, checking if requested days exceed available SERVICE CREDIT balance and storing the deficit immediately. Updated DLAppForLeaveController to populate cell B58 with day_debt value in Excel export. Added Day Debt column to admin leave_requests.blade.php, teacher dashboard, and approved-leave-requests PDF
</commit_message>
<xml_diff>
--- a/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
+++ b/resources/views/forms/LEAVE PLARIDEL CS-REVISED-2025 BLANK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\personal-info-management-system\resources\views\forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7350AE26-EBF7-4A43-BE62-9B0EFCF407ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E496E749-1DFB-4509-B303-8371B3CA2EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1410" windowWidth="29040" windowHeight="15720" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8FA0024E-7E78-4BAF-B796-907D8E8CF622}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1307,7 +1307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1387,6 +1387,69 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1438,67 +1501,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1871,8 +1877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27B6FB-8E85-4B80-9281-508316E41DF7}">
   <dimension ref="A1:WVX123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25:O25"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2920,121 +2926,121 @@
       <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="49"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="72"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="72"/>
-      <c r="O6" s="72"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="45"/>
     </row>
     <row r="9" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:15" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="75"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="75"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="75"/>
-      <c r="O10" s="75"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -3046,38 +3052,38 @@
       <c r="F11" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="76" t="s">
+      <c r="G11" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76" t="s">
+      <c r="H11" s="52"/>
+      <c r="I11" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="76"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76" t="s">
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="77"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="80"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="55"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="56"/>
     </row>
     <row r="13" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
@@ -3106,11 +3112,11 @@
       <c r="G14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="70"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
       <c r="M14" s="14"/>
       <c r="N14" s="6" t="s">
         <v>13</v>
@@ -3135,22 +3141,22 @@
     </row>
     <row r="16" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
-      <c r="M17" s="67"/>
-      <c r="N17" s="67"/>
-      <c r="O17" s="68"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="48"/>
     </row>
     <row r="18" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
@@ -3265,8 +3271,8 @@
         <v>28</v>
       </c>
       <c r="M25" s="21"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="71"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="44"/>
     </row>
     <row r="26" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8"/>
@@ -3375,8 +3381,8 @@
       <c r="E33" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="57"/>
       <c r="H33" s="22"/>
       <c r="I33" s="8"/>
       <c r="J33" s="20"/>
@@ -3424,9 +3430,9 @@
     </row>
     <row r="36" spans="2:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
       <c r="H36" s="22"/>
       <c r="I36" s="8"/>
       <c r="J36" s="20"/>
@@ -3452,32 +3458,32 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
-      <c r="E38" s="61">
+      <c r="E38" s="58">
         <v>45330</v>
       </c>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="59"/>
       <c r="H38" s="22"/>
-      <c r="I38" s="57"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="58"/>
-      <c r="L38" s="58"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="59"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="80"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="H39" s="22"/>
-      <c r="I39" s="63" t="s">
+      <c r="I39" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="64"/>
-      <c r="N39" s="64"/>
-      <c r="O39" s="65"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="62"/>
     </row>
     <row r="40" spans="2:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9"/>
@@ -3497,22 +3503,22 @@
     </row>
     <row r="41" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="66" t="s">
+      <c r="B42" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="67"/>
-      <c r="K42" s="67"/>
-      <c r="L42" s="67"/>
-      <c r="M42" s="67"/>
-      <c r="N42" s="67"/>
-      <c r="O42" s="68"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="48"/>
     </row>
     <row r="43" spans="2:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
@@ -3540,8 +3546,8 @@
       <c r="E45" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="69"/>
-      <c r="G45" s="69"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
       <c r="H45" s="21"/>
       <c r="I45" s="8"/>
       <c r="O45" s="22"/>
@@ -3630,31 +3636,31 @@
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
-      <c r="E53" s="55"/>
-      <c r="F53" s="55"/>
-      <c r="G53" s="55"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
       <c r="I53" s="8"/>
-      <c r="L53" s="55"/>
-      <c r="M53" s="55"/>
-      <c r="N53" s="55"/>
-      <c r="O53" s="56"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="77"/>
     </row>
     <row r="54" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
-      <c r="E54" s="47" t="s">
+      <c r="E54" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
       <c r="I54" s="38"/>
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
-      <c r="L54" s="47" t="s">
+      <c r="L54" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="M54" s="47"/>
-      <c r="N54" s="47"/>
-      <c r="O54" s="48"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="69"/>
     </row>
     <row r="55" spans="2:15" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9"/>
@@ -3692,9 +3698,9 @@
       <c r="O56" s="27"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="49"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="71"/>
+      <c r="D57" s="71"/>
       <c r="E57" s="21" t="s">
         <v>63</v>
       </c>
@@ -3704,9 +3710,9 @@
       <c r="O57" s="11"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="9"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="82"/>
       <c r="E58" s="21" t="s">
         <v>64</v>
       </c>
@@ -3733,22 +3739,22 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="50"/>
-      <c r="I61" s="50"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="50"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="71"/>
+      <c r="L61" s="71"/>
       <c r="O61" s="22"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
-      <c r="G62" s="51"/>
-      <c r="H62" s="51"/>
-      <c r="I62" s="51"/>
-      <c r="J62" s="51"/>
-      <c r="K62" s="51"/>
-      <c r="L62" s="51"/>
+      <c r="G62" s="72"/>
+      <c r="H62" s="72"/>
+      <c r="I62" s="72"/>
+      <c r="J62" s="72"/>
+      <c r="K62" s="72"/>
+      <c r="L62" s="72"/>
       <c r="O62" s="22"/>
     </row>
     <row r="63" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3774,731 +3780,731 @@
     <row r="68" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="52" t="s">
+      <c r="B70" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-      <c r="H70" s="53"/>
-      <c r="I70" s="53"/>
-      <c r="J70" s="53"/>
-      <c r="K70" s="53"/>
-      <c r="L70" s="53"/>
-      <c r="M70" s="53"/>
-      <c r="N70" s="53"/>
-      <c r="O70" s="54"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
+      <c r="E70" s="74"/>
+      <c r="F70" s="74"/>
+      <c r="G70" s="74"/>
+      <c r="H70" s="74"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
+      <c r="K70" s="74"/>
+      <c r="L70" s="74"/>
+      <c r="M70" s="74"/>
+      <c r="N70" s="74"/>
+      <c r="O70" s="75"/>
     </row>
     <row r="71" spans="2:15" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="64" t="s">
         <v>67</v>
       </c>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
-      <c r="E72" s="44"/>
-      <c r="F72" s="44"/>
-      <c r="G72" s="44"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="43" t="s">
+      <c r="C72" s="65"/>
+      <c r="D72" s="65"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="65"/>
+      <c r="G72" s="65"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="64" t="s">
         <v>68</v>
       </c>
-      <c r="J72" s="44"/>
-      <c r="K72" s="44"/>
-      <c r="L72" s="44"/>
-      <c r="M72" s="44"/>
-      <c r="N72" s="44"/>
-      <c r="O72" s="44"/>
+      <c r="J72" s="65"/>
+      <c r="K72" s="65"/>
+      <c r="L72" s="65"/>
+      <c r="M72" s="65"/>
+      <c r="N72" s="65"/>
+      <c r="O72" s="65"/>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="44"/>
-      <c r="C73" s="44"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="44"/>
-      <c r="F73" s="44"/>
-      <c r="G73" s="44"/>
-      <c r="H73" s="44"/>
-      <c r="I73" s="44"/>
-      <c r="J73" s="44"/>
-      <c r="K73" s="44"/>
-      <c r="L73" s="44"/>
-      <c r="M73" s="44"/>
-      <c r="N73" s="44"/>
-      <c r="O73" s="44"/>
+      <c r="B73" s="65"/>
+      <c r="C73" s="65"/>
+      <c r="D73" s="65"/>
+      <c r="E73" s="65"/>
+      <c r="F73" s="65"/>
+      <c r="G73" s="65"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="65"/>
+      <c r="J73" s="65"/>
+      <c r="K73" s="65"/>
+      <c r="L73" s="65"/>
+      <c r="M73" s="65"/>
+      <c r="N73" s="65"/>
+      <c r="O73" s="65"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="44"/>
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
-      <c r="E74" s="44"/>
-      <c r="F74" s="44"/>
-      <c r="G74" s="44"/>
-      <c r="H74" s="44"/>
-      <c r="I74" s="44"/>
-      <c r="J74" s="44"/>
-      <c r="K74" s="44"/>
-      <c r="L74" s="44"/>
-      <c r="M74" s="44"/>
-      <c r="N74" s="44"/>
-      <c r="O74" s="44"/>
+      <c r="B74" s="65"/>
+      <c r="C74" s="65"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="65"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="65"/>
+      <c r="J74" s="65"/>
+      <c r="K74" s="65"/>
+      <c r="L74" s="65"/>
+      <c r="M74" s="65"/>
+      <c r="N74" s="65"/>
+      <c r="O74" s="65"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="44"/>
-      <c r="C75" s="44"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="44"/>
-      <c r="J75" s="44"/>
-      <c r="K75" s="44"/>
-      <c r="L75" s="44"/>
-      <c r="M75" s="44"/>
-      <c r="N75" s="44"/>
-      <c r="O75" s="44"/>
+      <c r="B75" s="65"/>
+      <c r="C75" s="65"/>
+      <c r="D75" s="65"/>
+      <c r="E75" s="65"/>
+      <c r="F75" s="65"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="65"/>
+      <c r="J75" s="65"/>
+      <c r="K75" s="65"/>
+      <c r="L75" s="65"/>
+      <c r="M75" s="65"/>
+      <c r="N75" s="65"/>
+      <c r="O75" s="65"/>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="44"/>
-      <c r="C76" s="44"/>
-      <c r="D76" s="44"/>
-      <c r="E76" s="44"/>
-      <c r="F76" s="44"/>
-      <c r="G76" s="44"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="44"/>
-      <c r="J76" s="44"/>
-      <c r="K76" s="44"/>
-      <c r="L76" s="44"/>
-      <c r="M76" s="44"/>
-      <c r="N76" s="44"/>
-      <c r="O76" s="44"/>
+      <c r="B76" s="65"/>
+      <c r="C76" s="65"/>
+      <c r="D76" s="65"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="65"/>
+      <c r="G76" s="65"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
+      <c r="J76" s="65"/>
+      <c r="K76" s="65"/>
+      <c r="L76" s="65"/>
+      <c r="M76" s="65"/>
+      <c r="N76" s="65"/>
+      <c r="O76" s="65"/>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="44"/>
-      <c r="C77" s="44"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="44"/>
-      <c r="I77" s="44"/>
-      <c r="J77" s="44"/>
-      <c r="K77" s="44"/>
-      <c r="L77" s="44"/>
-      <c r="M77" s="44"/>
-      <c r="N77" s="44"/>
-      <c r="O77" s="44"/>
+      <c r="B77" s="65"/>
+      <c r="C77" s="65"/>
+      <c r="D77" s="65"/>
+      <c r="E77" s="65"/>
+      <c r="F77" s="65"/>
+      <c r="G77" s="65"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="65"/>
+      <c r="J77" s="65"/>
+      <c r="K77" s="65"/>
+      <c r="L77" s="65"/>
+      <c r="M77" s="65"/>
+      <c r="N77" s="65"/>
+      <c r="O77" s="65"/>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="44"/>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="44"/>
-      <c r="I78" s="44"/>
-      <c r="J78" s="44"/>
-      <c r="K78" s="44"/>
-      <c r="L78" s="44"/>
-      <c r="M78" s="44"/>
-      <c r="N78" s="44"/>
-      <c r="O78" s="44"/>
+      <c r="B78" s="65"/>
+      <c r="C78" s="65"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="65"/>
+      <c r="G78" s="65"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
+      <c r="J78" s="65"/>
+      <c r="K78" s="65"/>
+      <c r="L78" s="65"/>
+      <c r="M78" s="65"/>
+      <c r="N78" s="65"/>
+      <c r="O78" s="65"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="44"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="44"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="44"/>
-      <c r="J79" s="44"/>
-      <c r="K79" s="44"/>
-      <c r="L79" s="44"/>
-      <c r="M79" s="44"/>
-      <c r="N79" s="44"/>
-      <c r="O79" s="44"/>
+      <c r="B79" s="65"/>
+      <c r="C79" s="65"/>
+      <c r="D79" s="65"/>
+      <c r="E79" s="65"/>
+      <c r="F79" s="65"/>
+      <c r="G79" s="65"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="65"/>
+      <c r="J79" s="65"/>
+      <c r="K79" s="65"/>
+      <c r="L79" s="65"/>
+      <c r="M79" s="65"/>
+      <c r="N79" s="65"/>
+      <c r="O79" s="65"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="44"/>
-      <c r="C80" s="44"/>
-      <c r="D80" s="44"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="44"/>
-      <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="44"/>
-      <c r="K80" s="44"/>
-      <c r="L80" s="44"/>
-      <c r="M80" s="44"/>
-      <c r="N80" s="44"/>
-      <c r="O80" s="44"/>
+      <c r="B80" s="65"/>
+      <c r="C80" s="65"/>
+      <c r="D80" s="65"/>
+      <c r="E80" s="65"/>
+      <c r="F80" s="65"/>
+      <c r="G80" s="65"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
+      <c r="J80" s="65"/>
+      <c r="K80" s="65"/>
+      <c r="L80" s="65"/>
+      <c r="M80" s="65"/>
+      <c r="N80" s="65"/>
+      <c r="O80" s="65"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="44"/>
-      <c r="C81" s="44"/>
-      <c r="D81" s="44"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="44"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="44"/>
-      <c r="K81" s="44"/>
-      <c r="L81" s="44"/>
-      <c r="M81" s="44"/>
-      <c r="N81" s="44"/>
-      <c r="O81" s="44"/>
+      <c r="B81" s="65"/>
+      <c r="C81" s="65"/>
+      <c r="D81" s="65"/>
+      <c r="E81" s="65"/>
+      <c r="F81" s="65"/>
+      <c r="G81" s="65"/>
+      <c r="H81" s="65"/>
+      <c r="I81" s="65"/>
+      <c r="J81" s="65"/>
+      <c r="K81" s="65"/>
+      <c r="L81" s="65"/>
+      <c r="M81" s="65"/>
+      <c r="N81" s="65"/>
+      <c r="O81" s="65"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="44"/>
-      <c r="C82" s="44"/>
-      <c r="D82" s="44"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="44"/>
-      <c r="L82" s="44"/>
-      <c r="M82" s="44"/>
-      <c r="N82" s="44"/>
-      <c r="O82" s="44"/>
+      <c r="B82" s="65"/>
+      <c r="C82" s="65"/>
+      <c r="D82" s="65"/>
+      <c r="E82" s="65"/>
+      <c r="F82" s="65"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="65"/>
+      <c r="J82" s="65"/>
+      <c r="K82" s="65"/>
+      <c r="L82" s="65"/>
+      <c r="M82" s="65"/>
+      <c r="N82" s="65"/>
+      <c r="O82" s="65"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B83" s="44"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="44"/>
-      <c r="I83" s="44"/>
-      <c r="J83" s="44"/>
-      <c r="K83" s="44"/>
-      <c r="L83" s="44"/>
-      <c r="M83" s="44"/>
-      <c r="N83" s="44"/>
-      <c r="O83" s="44"/>
+      <c r="B83" s="65"/>
+      <c r="C83" s="65"/>
+      <c r="D83" s="65"/>
+      <c r="E83" s="65"/>
+      <c r="F83" s="65"/>
+      <c r="G83" s="65"/>
+      <c r="H83" s="65"/>
+      <c r="I83" s="65"/>
+      <c r="J83" s="65"/>
+      <c r="K83" s="65"/>
+      <c r="L83" s="65"/>
+      <c r="M83" s="65"/>
+      <c r="N83" s="65"/>
+      <c r="O83" s="65"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="44"/>
-      <c r="C84" s="44"/>
-      <c r="D84" s="44"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="44"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="44"/>
-      <c r="J84" s="44"/>
-      <c r="K84" s="44"/>
-      <c r="L84" s="44"/>
-      <c r="M84" s="44"/>
-      <c r="N84" s="44"/>
-      <c r="O84" s="44"/>
+      <c r="B84" s="65"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="65"/>
+      <c r="E84" s="65"/>
+      <c r="F84" s="65"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="65"/>
+      <c r="J84" s="65"/>
+      <c r="K84" s="65"/>
+      <c r="L84" s="65"/>
+      <c r="M84" s="65"/>
+      <c r="N84" s="65"/>
+      <c r="O84" s="65"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="44"/>
-      <c r="C85" s="44"/>
-      <c r="D85" s="44"/>
-      <c r="E85" s="44"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="44"/>
-      <c r="J85" s="44"/>
-      <c r="K85" s="44"/>
-      <c r="L85" s="44"/>
-      <c r="M85" s="44"/>
-      <c r="N85" s="44"/>
-      <c r="O85" s="44"/>
+      <c r="B85" s="65"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="65"/>
+      <c r="E85" s="65"/>
+      <c r="F85" s="65"/>
+      <c r="G85" s="65"/>
+      <c r="H85" s="65"/>
+      <c r="I85" s="65"/>
+      <c r="J85" s="65"/>
+      <c r="K85" s="65"/>
+      <c r="L85" s="65"/>
+      <c r="M85" s="65"/>
+      <c r="N85" s="65"/>
+      <c r="O85" s="65"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="44"/>
-      <c r="C86" s="44"/>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="44"/>
-      <c r="I86" s="44"/>
-      <c r="J86" s="44"/>
-      <c r="K86" s="44"/>
-      <c r="L86" s="44"/>
-      <c r="M86" s="44"/>
-      <c r="N86" s="44"/>
-      <c r="O86" s="44"/>
+      <c r="B86" s="65"/>
+      <c r="C86" s="65"/>
+      <c r="D86" s="65"/>
+      <c r="E86" s="65"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="65"/>
+      <c r="J86" s="65"/>
+      <c r="K86" s="65"/>
+      <c r="L86" s="65"/>
+      <c r="M86" s="65"/>
+      <c r="N86" s="65"/>
+      <c r="O86" s="65"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="44"/>
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="44"/>
-      <c r="I87" s="44"/>
-      <c r="J87" s="44"/>
-      <c r="K87" s="44"/>
-      <c r="L87" s="44"/>
-      <c r="M87" s="44"/>
-      <c r="N87" s="44"/>
-      <c r="O87" s="44"/>
+      <c r="B87" s="65"/>
+      <c r="C87" s="65"/>
+      <c r="D87" s="65"/>
+      <c r="E87" s="65"/>
+      <c r="F87" s="65"/>
+      <c r="G87" s="65"/>
+      <c r="H87" s="65"/>
+      <c r="I87" s="65"/>
+      <c r="J87" s="65"/>
+      <c r="K87" s="65"/>
+      <c r="L87" s="65"/>
+      <c r="M87" s="65"/>
+      <c r="N87" s="65"/>
+      <c r="O87" s="65"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="44"/>
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="44"/>
-      <c r="K88" s="44"/>
-      <c r="L88" s="44"/>
-      <c r="M88" s="44"/>
-      <c r="N88" s="44"/>
-      <c r="O88" s="44"/>
+      <c r="B88" s="65"/>
+      <c r="C88" s="65"/>
+      <c r="D88" s="65"/>
+      <c r="E88" s="65"/>
+      <c r="F88" s="65"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="65"/>
+      <c r="J88" s="65"/>
+      <c r="K88" s="65"/>
+      <c r="L88" s="65"/>
+      <c r="M88" s="65"/>
+      <c r="N88" s="65"/>
+      <c r="O88" s="65"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89" s="44"/>
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="44"/>
-      <c r="F89" s="44"/>
-      <c r="G89" s="44"/>
-      <c r="H89" s="44"/>
-      <c r="I89" s="44"/>
-      <c r="J89" s="44"/>
-      <c r="K89" s="44"/>
-      <c r="L89" s="44"/>
-      <c r="M89" s="44"/>
-      <c r="N89" s="44"/>
-      <c r="O89" s="44"/>
+      <c r="B89" s="65"/>
+      <c r="C89" s="65"/>
+      <c r="D89" s="65"/>
+      <c r="E89" s="65"/>
+      <c r="F89" s="65"/>
+      <c r="G89" s="65"/>
+      <c r="H89" s="65"/>
+      <c r="I89" s="65"/>
+      <c r="J89" s="65"/>
+      <c r="K89" s="65"/>
+      <c r="L89" s="65"/>
+      <c r="M89" s="65"/>
+      <c r="N89" s="65"/>
+      <c r="O89" s="65"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B90" s="44"/>
-      <c r="C90" s="44"/>
-      <c r="D90" s="44"/>
-      <c r="E90" s="44"/>
-      <c r="F90" s="44"/>
-      <c r="G90" s="44"/>
-      <c r="H90" s="44"/>
-      <c r="I90" s="44"/>
-      <c r="J90" s="44"/>
-      <c r="K90" s="44"/>
-      <c r="L90" s="44"/>
-      <c r="M90" s="44"/>
-      <c r="N90" s="44"/>
-      <c r="O90" s="44"/>
+      <c r="B90" s="65"/>
+      <c r="C90" s="65"/>
+      <c r="D90" s="65"/>
+      <c r="E90" s="65"/>
+      <c r="F90" s="65"/>
+      <c r="G90" s="65"/>
+      <c r="H90" s="65"/>
+      <c r="I90" s="65"/>
+      <c r="J90" s="65"/>
+      <c r="K90" s="65"/>
+      <c r="L90" s="65"/>
+      <c r="M90" s="65"/>
+      <c r="N90" s="65"/>
+      <c r="O90" s="65"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="44"/>
-      <c r="C91" s="44"/>
-      <c r="D91" s="44"/>
-      <c r="E91" s="44"/>
-      <c r="F91" s="44"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="44"/>
-      <c r="I91" s="44"/>
-      <c r="J91" s="44"/>
-      <c r="K91" s="44"/>
-      <c r="L91" s="44"/>
-      <c r="M91" s="44"/>
-      <c r="N91" s="44"/>
-      <c r="O91" s="44"/>
+      <c r="B91" s="65"/>
+      <c r="C91" s="65"/>
+      <c r="D91" s="65"/>
+      <c r="E91" s="65"/>
+      <c r="F91" s="65"/>
+      <c r="G91" s="65"/>
+      <c r="H91" s="65"/>
+      <c r="I91" s="65"/>
+      <c r="J91" s="65"/>
+      <c r="K91" s="65"/>
+      <c r="L91" s="65"/>
+      <c r="M91" s="65"/>
+      <c r="N91" s="65"/>
+      <c r="O91" s="65"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B92" s="44"/>
-      <c r="C92" s="44"/>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="44"/>
-      <c r="I92" s="44"/>
-      <c r="J92" s="44"/>
-      <c r="K92" s="44"/>
-      <c r="L92" s="44"/>
-      <c r="M92" s="44"/>
-      <c r="N92" s="44"/>
-      <c r="O92" s="44"/>
+      <c r="B92" s="65"/>
+      <c r="C92" s="65"/>
+      <c r="D92" s="65"/>
+      <c r="E92" s="65"/>
+      <c r="F92" s="65"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="65"/>
+      <c r="I92" s="65"/>
+      <c r="J92" s="65"/>
+      <c r="K92" s="65"/>
+      <c r="L92" s="65"/>
+      <c r="M92" s="65"/>
+      <c r="N92" s="65"/>
+      <c r="O92" s="65"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="44"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="44"/>
-      <c r="I93" s="44"/>
-      <c r="J93" s="44"/>
-      <c r="K93" s="44"/>
-      <c r="L93" s="44"/>
-      <c r="M93" s="44"/>
-      <c r="N93" s="44"/>
-      <c r="O93" s="44"/>
+      <c r="B93" s="65"/>
+      <c r="C93" s="65"/>
+      <c r="D93" s="65"/>
+      <c r="E93" s="65"/>
+      <c r="F93" s="65"/>
+      <c r="G93" s="65"/>
+      <c r="H93" s="65"/>
+      <c r="I93" s="65"/>
+      <c r="J93" s="65"/>
+      <c r="K93" s="65"/>
+      <c r="L93" s="65"/>
+      <c r="M93" s="65"/>
+      <c r="N93" s="65"/>
+      <c r="O93" s="65"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
-      <c r="D94" s="44"/>
-      <c r="E94" s="44"/>
-      <c r="F94" s="44"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="44"/>
-      <c r="J94" s="44"/>
-      <c r="K94" s="44"/>
-      <c r="L94" s="44"/>
-      <c r="M94" s="44"/>
-      <c r="N94" s="44"/>
-      <c r="O94" s="44"/>
+      <c r="B94" s="65"/>
+      <c r="C94" s="65"/>
+      <c r="D94" s="65"/>
+      <c r="E94" s="65"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="65"/>
+      <c r="H94" s="65"/>
+      <c r="I94" s="65"/>
+      <c r="J94" s="65"/>
+      <c r="K94" s="65"/>
+      <c r="L94" s="65"/>
+      <c r="M94" s="65"/>
+      <c r="N94" s="65"/>
+      <c r="O94" s="65"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="44"/>
-      <c r="C95" s="44"/>
-      <c r="D95" s="44"/>
-      <c r="E95" s="44"/>
-      <c r="F95" s="44"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="44"/>
-      <c r="I95" s="44"/>
-      <c r="J95" s="44"/>
-      <c r="K95" s="44"/>
-      <c r="L95" s="44"/>
-      <c r="M95" s="44"/>
-      <c r="N95" s="44"/>
-      <c r="O95" s="44"/>
+      <c r="B95" s="65"/>
+      <c r="C95" s="65"/>
+      <c r="D95" s="65"/>
+      <c r="E95" s="65"/>
+      <c r="F95" s="65"/>
+      <c r="G95" s="65"/>
+      <c r="H95" s="65"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="65"/>
+      <c r="L95" s="65"/>
+      <c r="M95" s="65"/>
+      <c r="N95" s="65"/>
+      <c r="O95" s="65"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B96" s="44"/>
-      <c r="C96" s="44"/>
-      <c r="D96" s="44"/>
-      <c r="E96" s="44"/>
-      <c r="F96" s="44"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="44"/>
-      <c r="I96" s="44"/>
-      <c r="J96" s="44"/>
-      <c r="K96" s="44"/>
-      <c r="L96" s="44"/>
-      <c r="M96" s="44"/>
-      <c r="N96" s="44"/>
-      <c r="O96" s="44"/>
+      <c r="B96" s="65"/>
+      <c r="C96" s="65"/>
+      <c r="D96" s="65"/>
+      <c r="E96" s="65"/>
+      <c r="F96" s="65"/>
+      <c r="G96" s="65"/>
+      <c r="H96" s="65"/>
+      <c r="I96" s="65"/>
+      <c r="J96" s="65"/>
+      <c r="K96" s="65"/>
+      <c r="L96" s="65"/>
+      <c r="M96" s="65"/>
+      <c r="N96" s="65"/>
+      <c r="O96" s="65"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97" s="44"/>
-      <c r="C97" s="44"/>
-      <c r="D97" s="44"/>
-      <c r="E97" s="44"/>
-      <c r="F97" s="44"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="44"/>
-      <c r="I97" s="44"/>
-      <c r="J97" s="44"/>
-      <c r="K97" s="44"/>
-      <c r="L97" s="44"/>
-      <c r="M97" s="44"/>
-      <c r="N97" s="44"/>
-      <c r="O97" s="44"/>
+      <c r="B97" s="65"/>
+      <c r="C97" s="65"/>
+      <c r="D97" s="65"/>
+      <c r="E97" s="65"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="65"/>
+      <c r="H97" s="65"/>
+      <c r="I97" s="65"/>
+      <c r="J97" s="65"/>
+      <c r="K97" s="65"/>
+      <c r="L97" s="65"/>
+      <c r="M97" s="65"/>
+      <c r="N97" s="65"/>
+      <c r="O97" s="65"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="44"/>
-      <c r="C98" s="44"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="44"/>
-      <c r="F98" s="44"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="44"/>
-      <c r="I98" s="44"/>
-      <c r="J98" s="44"/>
-      <c r="K98" s="44"/>
-      <c r="L98" s="44"/>
-      <c r="M98" s="44"/>
-      <c r="N98" s="44"/>
-      <c r="O98" s="44"/>
+      <c r="B98" s="65"/>
+      <c r="C98" s="65"/>
+      <c r="D98" s="65"/>
+      <c r="E98" s="65"/>
+      <c r="F98" s="65"/>
+      <c r="G98" s="65"/>
+      <c r="H98" s="65"/>
+      <c r="I98" s="65"/>
+      <c r="J98" s="65"/>
+      <c r="K98" s="65"/>
+      <c r="L98" s="65"/>
+      <c r="M98" s="65"/>
+      <c r="N98" s="65"/>
+      <c r="O98" s="65"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99" s="44"/>
-      <c r="C99" s="44"/>
-      <c r="D99" s="44"/>
-      <c r="E99" s="44"/>
-      <c r="F99" s="44"/>
-      <c r="G99" s="44"/>
-      <c r="H99" s="44"/>
-      <c r="I99" s="44"/>
-      <c r="J99" s="44"/>
-      <c r="K99" s="44"/>
-      <c r="L99" s="44"/>
-      <c r="M99" s="44"/>
-      <c r="N99" s="44"/>
-      <c r="O99" s="44"/>
+      <c r="B99" s="65"/>
+      <c r="C99" s="65"/>
+      <c r="D99" s="65"/>
+      <c r="E99" s="65"/>
+      <c r="F99" s="65"/>
+      <c r="G99" s="65"/>
+      <c r="H99" s="65"/>
+      <c r="I99" s="65"/>
+      <c r="J99" s="65"/>
+      <c r="K99" s="65"/>
+      <c r="L99" s="65"/>
+      <c r="M99" s="65"/>
+      <c r="N99" s="65"/>
+      <c r="O99" s="65"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-      <c r="E100" s="44"/>
-      <c r="F100" s="44"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="44"/>
-      <c r="I100" s="44"/>
-      <c r="J100" s="44"/>
-      <c r="K100" s="44"/>
-      <c r="L100" s="44"/>
-      <c r="M100" s="44"/>
-      <c r="N100" s="44"/>
-      <c r="O100" s="44"/>
+      <c r="B100" s="65"/>
+      <c r="C100" s="65"/>
+      <c r="D100" s="65"/>
+      <c r="E100" s="65"/>
+      <c r="F100" s="65"/>
+      <c r="G100" s="65"/>
+      <c r="H100" s="65"/>
+      <c r="I100" s="65"/>
+      <c r="J100" s="65"/>
+      <c r="K100" s="65"/>
+      <c r="L100" s="65"/>
+      <c r="M100" s="65"/>
+      <c r="N100" s="65"/>
+      <c r="O100" s="65"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="44"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-      <c r="E101" s="44"/>
-      <c r="F101" s="44"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="44"/>
-      <c r="I101" s="44"/>
-      <c r="J101" s="44"/>
-      <c r="K101" s="44"/>
-      <c r="L101" s="44"/>
-      <c r="M101" s="44"/>
-      <c r="N101" s="44"/>
-      <c r="O101" s="44"/>
+      <c r="B101" s="65"/>
+      <c r="C101" s="65"/>
+      <c r="D101" s="65"/>
+      <c r="E101" s="65"/>
+      <c r="F101" s="65"/>
+      <c r="G101" s="65"/>
+      <c r="H101" s="65"/>
+      <c r="I101" s="65"/>
+      <c r="J101" s="65"/>
+      <c r="K101" s="65"/>
+      <c r="L101" s="65"/>
+      <c r="M101" s="65"/>
+      <c r="N101" s="65"/>
+      <c r="O101" s="65"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B102" s="44"/>
-      <c r="C102" s="44"/>
-      <c r="D102" s="44"/>
-      <c r="E102" s="44"/>
-      <c r="F102" s="44"/>
-      <c r="G102" s="44"/>
-      <c r="H102" s="44"/>
-      <c r="I102" s="44"/>
-      <c r="J102" s="44"/>
-      <c r="K102" s="44"/>
-      <c r="L102" s="44"/>
-      <c r="M102" s="44"/>
-      <c r="N102" s="44"/>
-      <c r="O102" s="44"/>
+      <c r="B102" s="65"/>
+      <c r="C102" s="65"/>
+      <c r="D102" s="65"/>
+      <c r="E102" s="65"/>
+      <c r="F102" s="65"/>
+      <c r="G102" s="65"/>
+      <c r="H102" s="65"/>
+      <c r="I102" s="65"/>
+      <c r="J102" s="65"/>
+      <c r="K102" s="65"/>
+      <c r="L102" s="65"/>
+      <c r="M102" s="65"/>
+      <c r="N102" s="65"/>
+      <c r="O102" s="65"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B103" s="44"/>
-      <c r="C103" s="44"/>
-      <c r="D103" s="44"/>
-      <c r="E103" s="44"/>
-      <c r="F103" s="44"/>
-      <c r="G103" s="44"/>
-      <c r="H103" s="44"/>
-      <c r="I103" s="44"/>
-      <c r="J103" s="44"/>
-      <c r="K103" s="44"/>
-      <c r="L103" s="44"/>
-      <c r="M103" s="44"/>
-      <c r="N103" s="44"/>
-      <c r="O103" s="44"/>
+      <c r="B103" s="65"/>
+      <c r="C103" s="65"/>
+      <c r="D103" s="65"/>
+      <c r="E103" s="65"/>
+      <c r="F103" s="65"/>
+      <c r="G103" s="65"/>
+      <c r="H103" s="65"/>
+      <c r="I103" s="65"/>
+      <c r="J103" s="65"/>
+      <c r="K103" s="65"/>
+      <c r="L103" s="65"/>
+      <c r="M103" s="65"/>
+      <c r="N103" s="65"/>
+      <c r="O103" s="65"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104" s="44"/>
-      <c r="C104" s="44"/>
-      <c r="D104" s="44"/>
-      <c r="E104" s="44"/>
-      <c r="F104" s="44"/>
-      <c r="G104" s="44"/>
-      <c r="H104" s="44"/>
-      <c r="I104" s="44"/>
-      <c r="J104" s="44"/>
-      <c r="K104" s="44"/>
-      <c r="L104" s="44"/>
-      <c r="M104" s="44"/>
-      <c r="N104" s="44"/>
-      <c r="O104" s="44"/>
+      <c r="B104" s="65"/>
+      <c r="C104" s="65"/>
+      <c r="D104" s="65"/>
+      <c r="E104" s="65"/>
+      <c r="F104" s="65"/>
+      <c r="G104" s="65"/>
+      <c r="H104" s="65"/>
+      <c r="I104" s="65"/>
+      <c r="J104" s="65"/>
+      <c r="K104" s="65"/>
+      <c r="L104" s="65"/>
+      <c r="M104" s="65"/>
+      <c r="N104" s="65"/>
+      <c r="O104" s="65"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105" s="44"/>
-      <c r="C105" s="44"/>
-      <c r="D105" s="44"/>
-      <c r="E105" s="44"/>
-      <c r="F105" s="44"/>
-      <c r="G105" s="44"/>
-      <c r="H105" s="44"/>
-      <c r="I105" s="44"/>
-      <c r="J105" s="44"/>
-      <c r="K105" s="44"/>
-      <c r="L105" s="44"/>
-      <c r="M105" s="44"/>
-      <c r="N105" s="44"/>
-      <c r="O105" s="44"/>
+      <c r="B105" s="65"/>
+      <c r="C105" s="65"/>
+      <c r="D105" s="65"/>
+      <c r="E105" s="65"/>
+      <c r="F105" s="65"/>
+      <c r="G105" s="65"/>
+      <c r="H105" s="65"/>
+      <c r="I105" s="65"/>
+      <c r="J105" s="65"/>
+      <c r="K105" s="65"/>
+      <c r="L105" s="65"/>
+      <c r="M105" s="65"/>
+      <c r="N105" s="65"/>
+      <c r="O105" s="65"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B106" s="44"/>
-      <c r="C106" s="44"/>
-      <c r="D106" s="44"/>
-      <c r="E106" s="44"/>
-      <c r="F106" s="44"/>
-      <c r="G106" s="44"/>
-      <c r="H106" s="44"/>
-      <c r="I106" s="44"/>
-      <c r="J106" s="44"/>
-      <c r="K106" s="44"/>
-      <c r="L106" s="44"/>
-      <c r="M106" s="44"/>
-      <c r="N106" s="44"/>
-      <c r="O106" s="44"/>
+      <c r="B106" s="65"/>
+      <c r="C106" s="65"/>
+      <c r="D106" s="65"/>
+      <c r="E106" s="65"/>
+      <c r="F106" s="65"/>
+      <c r="G106" s="65"/>
+      <c r="H106" s="65"/>
+      <c r="I106" s="65"/>
+      <c r="J106" s="65"/>
+      <c r="K106" s="65"/>
+      <c r="L106" s="65"/>
+      <c r="M106" s="65"/>
+      <c r="N106" s="65"/>
+      <c r="O106" s="65"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="44"/>
-      <c r="C107" s="44"/>
-      <c r="D107" s="44"/>
-      <c r="E107" s="44"/>
-      <c r="F107" s="44"/>
-      <c r="G107" s="44"/>
-      <c r="H107" s="44"/>
-      <c r="I107" s="44"/>
-      <c r="J107" s="44"/>
-      <c r="K107" s="44"/>
-      <c r="L107" s="44"/>
-      <c r="M107" s="44"/>
-      <c r="N107" s="44"/>
-      <c r="O107" s="44"/>
+      <c r="B107" s="65"/>
+      <c r="C107" s="65"/>
+      <c r="D107" s="65"/>
+      <c r="E107" s="65"/>
+      <c r="F107" s="65"/>
+      <c r="G107" s="65"/>
+      <c r="H107" s="65"/>
+      <c r="I107" s="65"/>
+      <c r="J107" s="65"/>
+      <c r="K107" s="65"/>
+      <c r="L107" s="65"/>
+      <c r="M107" s="65"/>
+      <c r="N107" s="65"/>
+      <c r="O107" s="65"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="44"/>
-      <c r="C108" s="44"/>
-      <c r="D108" s="44"/>
-      <c r="E108" s="44"/>
-      <c r="F108" s="44"/>
-      <c r="G108" s="44"/>
-      <c r="H108" s="44"/>
-      <c r="I108" s="44"/>
-      <c r="J108" s="44"/>
-      <c r="K108" s="44"/>
-      <c r="L108" s="44"/>
-      <c r="M108" s="44"/>
-      <c r="N108" s="44"/>
-      <c r="O108" s="44"/>
+      <c r="B108" s="65"/>
+      <c r="C108" s="65"/>
+      <c r="D108" s="65"/>
+      <c r="E108" s="65"/>
+      <c r="F108" s="65"/>
+      <c r="G108" s="65"/>
+      <c r="H108" s="65"/>
+      <c r="I108" s="65"/>
+      <c r="J108" s="65"/>
+      <c r="K108" s="65"/>
+      <c r="L108" s="65"/>
+      <c r="M108" s="65"/>
+      <c r="N108" s="65"/>
+      <c r="O108" s="65"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B109" s="44"/>
-      <c r="C109" s="44"/>
-      <c r="D109" s="44"/>
-      <c r="E109" s="44"/>
-      <c r="F109" s="44"/>
-      <c r="G109" s="44"/>
-      <c r="H109" s="44"/>
-      <c r="I109" s="44"/>
-      <c r="J109" s="44"/>
-      <c r="K109" s="44"/>
-      <c r="L109" s="44"/>
-      <c r="M109" s="44"/>
-      <c r="N109" s="44"/>
-      <c r="O109" s="44"/>
+      <c r="B109" s="65"/>
+      <c r="C109" s="65"/>
+      <c r="D109" s="65"/>
+      <c r="E109" s="65"/>
+      <c r="F109" s="65"/>
+      <c r="G109" s="65"/>
+      <c r="H109" s="65"/>
+      <c r="I109" s="65"/>
+      <c r="J109" s="65"/>
+      <c r="K109" s="65"/>
+      <c r="L109" s="65"/>
+      <c r="M109" s="65"/>
+      <c r="N109" s="65"/>
+      <c r="O109" s="65"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B110" s="44"/>
-      <c r="C110" s="44"/>
-      <c r="D110" s="44"/>
-      <c r="E110" s="44"/>
-      <c r="F110" s="44"/>
-      <c r="G110" s="44"/>
-      <c r="H110" s="44"/>
-      <c r="I110" s="44"/>
-      <c r="J110" s="44"/>
-      <c r="K110" s="44"/>
-      <c r="L110" s="44"/>
-      <c r="M110" s="44"/>
-      <c r="N110" s="44"/>
-      <c r="O110" s="44"/>
+      <c r="B110" s="65"/>
+      <c r="C110" s="65"/>
+      <c r="D110" s="65"/>
+      <c r="E110" s="65"/>
+      <c r="F110" s="65"/>
+      <c r="G110" s="65"/>
+      <c r="H110" s="65"/>
+      <c r="I110" s="65"/>
+      <c r="J110" s="65"/>
+      <c r="K110" s="65"/>
+      <c r="L110" s="65"/>
+      <c r="M110" s="65"/>
+      <c r="N110" s="65"/>
+      <c r="O110" s="65"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B111" s="44"/>
-      <c r="C111" s="44"/>
-      <c r="D111" s="44"/>
-      <c r="E111" s="44"/>
-      <c r="F111" s="44"/>
-      <c r="G111" s="44"/>
-      <c r="H111" s="44"/>
-      <c r="I111" s="44"/>
-      <c r="J111" s="44"/>
-      <c r="K111" s="44"/>
-      <c r="L111" s="44"/>
-      <c r="M111" s="44"/>
-      <c r="N111" s="44"/>
-      <c r="O111" s="44"/>
+      <c r="B111" s="65"/>
+      <c r="C111" s="65"/>
+      <c r="D111" s="65"/>
+      <c r="E111" s="65"/>
+      <c r="F111" s="65"/>
+      <c r="G111" s="65"/>
+      <c r="H111" s="65"/>
+      <c r="I111" s="65"/>
+      <c r="J111" s="65"/>
+      <c r="K111" s="65"/>
+      <c r="L111" s="65"/>
+      <c r="M111" s="65"/>
+      <c r="N111" s="65"/>
+      <c r="O111" s="65"/>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B112" s="44"/>
-      <c r="C112" s="44"/>
-      <c r="D112" s="44"/>
-      <c r="E112" s="44"/>
-      <c r="F112" s="44"/>
-      <c r="G112" s="44"/>
-      <c r="H112" s="44"/>
-      <c r="I112" s="44"/>
-      <c r="J112" s="44"/>
-      <c r="K112" s="44"/>
-      <c r="L112" s="44"/>
-      <c r="M112" s="44"/>
-      <c r="N112" s="44"/>
-      <c r="O112" s="44"/>
+      <c r="B112" s="65"/>
+      <c r="C112" s="65"/>
+      <c r="D112" s="65"/>
+      <c r="E112" s="65"/>
+      <c r="F112" s="65"/>
+      <c r="G112" s="65"/>
+      <c r="H112" s="65"/>
+      <c r="I112" s="65"/>
+      <c r="J112" s="65"/>
+      <c r="K112" s="65"/>
+      <c r="L112" s="65"/>
+      <c r="M112" s="65"/>
+      <c r="N112" s="65"/>
+      <c r="O112" s="65"/>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="44"/>
-      <c r="C113" s="44"/>
-      <c r="D113" s="44"/>
-      <c r="E113" s="44"/>
-      <c r="F113" s="44"/>
-      <c r="G113" s="44"/>
-      <c r="H113" s="44"/>
-      <c r="I113" s="44"/>
-      <c r="J113" s="44"/>
-      <c r="K113" s="44"/>
-      <c r="L113" s="44"/>
-      <c r="M113" s="44"/>
-      <c r="N113" s="44"/>
-      <c r="O113" s="44"/>
+      <c r="B113" s="65"/>
+      <c r="C113" s="65"/>
+      <c r="D113" s="65"/>
+      <c r="E113" s="65"/>
+      <c r="F113" s="65"/>
+      <c r="G113" s="65"/>
+      <c r="H113" s="65"/>
+      <c r="I113" s="65"/>
+      <c r="J113" s="65"/>
+      <c r="K113" s="65"/>
+      <c r="L113" s="65"/>
+      <c r="M113" s="65"/>
+      <c r="N113" s="65"/>
+      <c r="O113" s="65"/>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="44"/>
-      <c r="C114" s="44"/>
-      <c r="D114" s="44"/>
-      <c r="E114" s="44"/>
-      <c r="F114" s="44"/>
-      <c r="G114" s="44"/>
-      <c r="H114" s="44"/>
-      <c r="I114" s="44"/>
-      <c r="J114" s="44"/>
-      <c r="K114" s="44"/>
-      <c r="L114" s="44"/>
-      <c r="M114" s="44"/>
-      <c r="N114" s="44"/>
-      <c r="O114" s="44"/>
+      <c r="B114" s="65"/>
+      <c r="C114" s="65"/>
+      <c r="D114" s="65"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="65"/>
+      <c r="G114" s="65"/>
+      <c r="H114" s="65"/>
+      <c r="I114" s="65"/>
+      <c r="J114" s="65"/>
+      <c r="K114" s="65"/>
+      <c r="L114" s="65"/>
+      <c r="M114" s="65"/>
+      <c r="N114" s="65"/>
+      <c r="O114" s="65"/>
     </row>
     <row r="115" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="44"/>
-      <c r="C115" s="44"/>
-      <c r="D115" s="44"/>
-      <c r="E115" s="44"/>
-      <c r="F115" s="44"/>
-      <c r="G115" s="44"/>
-      <c r="H115" s="44"/>
-      <c r="I115" s="44"/>
-      <c r="J115" s="44"/>
-      <c r="K115" s="44"/>
-      <c r="L115" s="44"/>
-      <c r="M115" s="44"/>
-      <c r="N115" s="44"/>
-      <c r="O115" s="44"/>
+      <c r="B115" s="65"/>
+      <c r="C115" s="65"/>
+      <c r="D115" s="65"/>
+      <c r="E115" s="65"/>
+      <c r="F115" s="65"/>
+      <c r="G115" s="65"/>
+      <c r="H115" s="65"/>
+      <c r="I115" s="65"/>
+      <c r="J115" s="65"/>
+      <c r="K115" s="65"/>
+      <c r="L115" s="65"/>
+      <c r="M115" s="65"/>
+      <c r="N115" s="65"/>
+      <c r="O115" s="65"/>
     </row>
     <row r="116" spans="2:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="40"/>
@@ -4518,45 +4524,64 @@
     </row>
     <row r="117" spans="2:15" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B118" s="45" t="s">
+      <c r="B118" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C118" s="45"/>
-      <c r="D118" s="45"/>
-      <c r="E118" s="45"/>
-      <c r="F118" s="45"/>
-      <c r="G118" s="45"/>
-      <c r="H118" s="45"/>
-      <c r="I118" s="45"/>
-      <c r="J118" s="45"/>
-      <c r="K118" s="45"/>
-      <c r="L118" s="45"/>
-      <c r="M118" s="45"/>
-      <c r="N118" s="45"/>
-      <c r="O118" s="45"/>
+      <c r="C118" s="66"/>
+      <c r="D118" s="66"/>
+      <c r="E118" s="66"/>
+      <c r="F118" s="66"/>
+      <c r="G118" s="66"/>
+      <c r="H118" s="66"/>
+      <c r="I118" s="66"/>
+      <c r="J118" s="66"/>
+      <c r="K118" s="66"/>
+      <c r="L118" s="66"/>
+      <c r="M118" s="66"/>
+      <c r="N118" s="66"/>
+      <c r="O118" s="66"/>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B119" s="45"/>
-      <c r="C119" s="45"/>
-      <c r="D119" s="45"/>
-      <c r="E119" s="45"/>
-      <c r="F119" s="45"/>
-      <c r="G119" s="45"/>
-      <c r="H119" s="45"/>
-      <c r="I119" s="45"/>
-      <c r="J119" s="45"/>
-      <c r="K119" s="45"/>
-      <c r="L119" s="45"/>
-      <c r="M119" s="45"/>
-      <c r="N119" s="45"/>
-      <c r="O119" s="45"/>
+      <c r="B119" s="66"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="66"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="66"/>
+      <c r="G119" s="66"/>
+      <c r="H119" s="66"/>
+      <c r="I119" s="66"/>
+      <c r="J119" s="66"/>
+      <c r="K119" s="66"/>
+      <c r="L119" s="66"/>
+      <c r="M119" s="66"/>
+      <c r="N119" s="66"/>
+      <c r="O119" s="66"/>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25"/>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
+    <mergeCell ref="B72:H115"/>
+    <mergeCell ref="I72:O115"/>
+    <mergeCell ref="B118:O119"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="L54:O54"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="G61:L61"/>
+    <mergeCell ref="G62:L62"/>
+    <mergeCell ref="B70:O70"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="L53:O53"/>
+    <mergeCell ref="I38:O38"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="I39:O39"/>
+    <mergeCell ref="B42:O42"/>
+    <mergeCell ref="F45:G45"/>
     <mergeCell ref="N25:O25"/>
     <mergeCell ref="A6:O6"/>
     <mergeCell ref="B17:O17"/>
@@ -4573,24 +4598,6 @@
     <mergeCell ref="I12:M12"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="H14:L14"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="I39:O39"/>
-    <mergeCell ref="B42:O42"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="B72:H115"/>
-    <mergeCell ref="I72:O115"/>
-    <mergeCell ref="B118:O119"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="L54:O54"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="G61:L61"/>
-    <mergeCell ref="G62:L62"/>
-    <mergeCell ref="B70:O70"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="L53:O53"/>
-    <mergeCell ref="I38:O38"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>